<commit_message>
Remoção de parametros desnecessários no applyMetricFilter()
</commit_message>
<xml_diff>
--- a/ES-2Sem-2021-Grupo-5_metricas.xlsx
+++ b/ES-2Sem-2021-Grupo-5_metricas.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="73">
   <si>
     <t>MethodID</t>
   </si>
@@ -164,7 +164,10 @@
     <t>getMaestro()</t>
   </si>
   <si>
-    <t>getMethodName(String s, String[] line)</t>
+    <t>getMethodName(Stack&lt;String&gt; stack)</t>
+  </si>
+  <si>
+    <t>getMetricName()</t>
   </si>
   <si>
     <t>getPackageClassName()</t>
@@ -177,12 +180,6 @@
   </si>
   <si>
     <t>handleOpenBracket()</t>
-  </si>
-  <si>
-    <t>isClass(String s)</t>
-  </si>
-  <si>
-    <t>positionArray(String[] line, String s)</t>
   </si>
   <si>
     <t>setPackageClassName(String packageClassName)</t>
@@ -336,7 +333,7 @@
         <v>7.0</v>
       </c>
       <c r="F2" t="n">
-        <v>238.0</v>
+        <v>237.0</v>
       </c>
       <c r="G2" t="n">
         <v>11.0</v>
@@ -371,7 +368,7 @@
         <v>7.0</v>
       </c>
       <c r="F3" t="n">
-        <v>238.0</v>
+        <v>237.0</v>
       </c>
       <c r="G3" t="n">
         <v>11.0</v>
@@ -406,7 +403,7 @@
         <v>7.0</v>
       </c>
       <c r="F4" t="n">
-        <v>238.0</v>
+        <v>237.0</v>
       </c>
       <c r="G4" t="n">
         <v>11.0</v>
@@ -441,7 +438,7 @@
         <v>7.0</v>
       </c>
       <c r="F5" t="n">
-        <v>238.0</v>
+        <v>237.0</v>
       </c>
       <c r="G5" t="n">
         <v>11.0</v>
@@ -450,7 +447,7 @@
         <v>1</v>
       </c>
       <c r="I5" t="n">
-        <v>127.0</v>
+        <v>126.0</v>
       </c>
       <c r="J5" t="n">
         <v>4.0</v>
@@ -476,7 +473,7 @@
         <v>7.0</v>
       </c>
       <c r="F6" t="n">
-        <v>238.0</v>
+        <v>237.0</v>
       </c>
       <c r="G6" t="n">
         <v>11.0</v>
@@ -511,7 +508,7 @@
         <v>7.0</v>
       </c>
       <c r="F7" t="n">
-        <v>238.0</v>
+        <v>237.0</v>
       </c>
       <c r="G7" t="n">
         <v>11.0</v>
@@ -546,7 +543,7 @@
         <v>7.0</v>
       </c>
       <c r="F8" t="n">
-        <v>238.0</v>
+        <v>237.0</v>
       </c>
       <c r="G8" t="n">
         <v>11.0</v>
@@ -581,7 +578,7 @@
         <v>3.0</v>
       </c>
       <c r="F9" t="n">
-        <v>33.0</v>
+        <v>34.0</v>
       </c>
       <c r="G9" t="n">
         <v>5.0</v>
@@ -590,7 +587,7 @@
         <v>1</v>
       </c>
       <c r="I9" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="J9" t="n">
         <v>0.0</v>
@@ -616,7 +613,7 @@
         <v>3.0</v>
       </c>
       <c r="F10" t="n">
-        <v>33.0</v>
+        <v>34.0</v>
       </c>
       <c r="G10" t="n">
         <v>5.0</v>
@@ -651,7 +648,7 @@
         <v>3.0</v>
       </c>
       <c r="F11" t="n">
-        <v>33.0</v>
+        <v>34.0</v>
       </c>
       <c r="G11" t="n">
         <v>5.0</v>
@@ -686,7 +683,7 @@
         <v>4.0</v>
       </c>
       <c r="F12" t="n">
-        <v>36.0</v>
+        <v>37.0</v>
       </c>
       <c r="G12" t="n">
         <v>4.0</v>
@@ -695,7 +692,7 @@
         <v>1</v>
       </c>
       <c r="I12" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="J12" t="n">
         <v>0.0</v>
@@ -721,7 +718,7 @@
         <v>4.0</v>
       </c>
       <c r="F13" t="n">
-        <v>36.0</v>
+        <v>37.0</v>
       </c>
       <c r="G13" t="n">
         <v>4.0</v>
@@ -756,7 +753,7 @@
         <v>4.0</v>
       </c>
       <c r="F14" t="n">
-        <v>36.0</v>
+        <v>37.0</v>
       </c>
       <c r="G14" t="n">
         <v>4.0</v>
@@ -791,7 +788,7 @@
         <v>4.0</v>
       </c>
       <c r="F15" t="n">
-        <v>36.0</v>
+        <v>37.0</v>
       </c>
       <c r="G15" t="n">
         <v>4.0</v>
@@ -835,7 +832,7 @@
         <v>1</v>
       </c>
       <c r="I16" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="J16" t="n">
         <v>0.0</v>
@@ -870,7 +867,7 @@
         <v>1</v>
       </c>
       <c r="I17" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="J17" t="n">
         <v>1.0</v>
@@ -931,7 +928,7 @@
         <v>18.0</v>
       </c>
       <c r="F19" t="n">
-        <v>172.0</v>
+        <v>174.0</v>
       </c>
       <c r="G19" t="n">
         <v>13.0</v>
@@ -966,7 +963,7 @@
         <v>18.0</v>
       </c>
       <c r="F20" t="n">
-        <v>172.0</v>
+        <v>174.0</v>
       </c>
       <c r="G20" t="n">
         <v>13.0</v>
@@ -1001,7 +998,7 @@
         <v>18.0</v>
       </c>
       <c r="F21" t="n">
-        <v>172.0</v>
+        <v>174.0</v>
       </c>
       <c r="G21" t="n">
         <v>13.0</v>
@@ -1036,7 +1033,7 @@
         <v>18.0</v>
       </c>
       <c r="F22" t="n">
-        <v>172.0</v>
+        <v>174.0</v>
       </c>
       <c r="G22" t="n">
         <v>13.0</v>
@@ -1045,7 +1042,7 @@
         <v>1</v>
       </c>
       <c r="I22" t="n">
-        <v>10.0</v>
+        <v>12.0</v>
       </c>
       <c r="J22" t="n">
         <v>1.0</v>
@@ -1071,7 +1068,7 @@
         <v>18.0</v>
       </c>
       <c r="F23" t="n">
-        <v>172.0</v>
+        <v>174.0</v>
       </c>
       <c r="G23" t="n">
         <v>13.0</v>
@@ -1106,7 +1103,7 @@
         <v>18.0</v>
       </c>
       <c r="F24" t="n">
-        <v>172.0</v>
+        <v>174.0</v>
       </c>
       <c r="G24" t="n">
         <v>13.0</v>
@@ -1141,7 +1138,7 @@
         <v>18.0</v>
       </c>
       <c r="F25" t="n">
-        <v>172.0</v>
+        <v>174.0</v>
       </c>
       <c r="G25" t="n">
         <v>13.0</v>
@@ -1176,7 +1173,7 @@
         <v>18.0</v>
       </c>
       <c r="F26" t="n">
-        <v>172.0</v>
+        <v>174.0</v>
       </c>
       <c r="G26" t="n">
         <v>13.0</v>
@@ -1211,7 +1208,7 @@
         <v>18.0</v>
       </c>
       <c r="F27" t="n">
-        <v>172.0</v>
+        <v>174.0</v>
       </c>
       <c r="G27" t="n">
         <v>13.0</v>
@@ -1246,7 +1243,7 @@
         <v>18.0</v>
       </c>
       <c r="F28" t="n">
-        <v>172.0</v>
+        <v>174.0</v>
       </c>
       <c r="G28" t="n">
         <v>13.0</v>
@@ -1281,7 +1278,7 @@
         <v>18.0</v>
       </c>
       <c r="F29" t="n">
-        <v>172.0</v>
+        <v>174.0</v>
       </c>
       <c r="G29" t="n">
         <v>13.0</v>
@@ -1316,7 +1313,7 @@
         <v>18.0</v>
       </c>
       <c r="F30" t="n">
-        <v>172.0</v>
+        <v>174.0</v>
       </c>
       <c r="G30" t="n">
         <v>13.0</v>
@@ -1351,7 +1348,7 @@
         <v>18.0</v>
       </c>
       <c r="F31" t="n">
-        <v>172.0</v>
+        <v>174.0</v>
       </c>
       <c r="G31" t="n">
         <v>13.0</v>
@@ -1386,7 +1383,7 @@
         <v>18.0</v>
       </c>
       <c r="F32" t="n">
-        <v>172.0</v>
+        <v>174.0</v>
       </c>
       <c r="G32" t="n">
         <v>13.0</v>
@@ -1421,7 +1418,7 @@
         <v>18.0</v>
       </c>
       <c r="F33" t="n">
-        <v>172.0</v>
+        <v>174.0</v>
       </c>
       <c r="G33" t="n">
         <v>13.0</v>
@@ -1456,7 +1453,7 @@
         <v>18.0</v>
       </c>
       <c r="F34" t="n">
-        <v>172.0</v>
+        <v>174.0</v>
       </c>
       <c r="G34" t="n">
         <v>13.0</v>
@@ -1491,7 +1488,7 @@
         <v>18.0</v>
       </c>
       <c r="F35" t="n">
-        <v>172.0</v>
+        <v>174.0</v>
       </c>
       <c r="G35" t="n">
         <v>13.0</v>
@@ -1526,7 +1523,7 @@
         <v>18.0</v>
       </c>
       <c r="F36" t="n">
-        <v>172.0</v>
+        <v>174.0</v>
       </c>
       <c r="G36" t="n">
         <v>13.0</v>
@@ -1558,13 +1555,13 @@
         <v>47</v>
       </c>
       <c r="E37" t="n">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
       <c r="F37" t="n">
-        <v>171.0</v>
+        <v>162.0</v>
       </c>
       <c r="G37" t="n">
-        <v>27.0</v>
+        <v>23.0</v>
       </c>
       <c r="H37" t="b">
         <v>1</v>
@@ -1593,19 +1590,19 @@
         <v>25</v>
       </c>
       <c r="E38" t="n">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
       <c r="F38" t="n">
-        <v>171.0</v>
+        <v>162.0</v>
       </c>
       <c r="G38" t="n">
-        <v>27.0</v>
+        <v>23.0</v>
       </c>
       <c r="H38" t="b">
         <v>1</v>
       </c>
       <c r="I38" t="n">
-        <v>37.0</v>
+        <v>38.0</v>
       </c>
       <c r="J38" t="n">
         <v>8.0</v>
@@ -1628,13 +1625,13 @@
         <v>48</v>
       </c>
       <c r="E39" t="n">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
       <c r="F39" t="n">
-        <v>171.0</v>
+        <v>162.0</v>
       </c>
       <c r="G39" t="n">
-        <v>27.0</v>
+        <v>23.0</v>
       </c>
       <c r="H39" t="b">
         <v>1</v>
@@ -1663,13 +1660,13 @@
         <v>49</v>
       </c>
       <c r="E40" t="n">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
       <c r="F40" t="n">
-        <v>171.0</v>
+        <v>162.0</v>
       </c>
       <c r="G40" t="n">
-        <v>27.0</v>
+        <v>23.0</v>
       </c>
       <c r="H40" t="b">
         <v>1</v>
@@ -1698,22 +1695,22 @@
         <v>50</v>
       </c>
       <c r="E41" t="n">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
       <c r="F41" t="n">
-        <v>171.0</v>
+        <v>162.0</v>
       </c>
       <c r="G41" t="n">
-        <v>27.0</v>
+        <v>23.0</v>
       </c>
       <c r="H41" t="b">
         <v>1</v>
       </c>
       <c r="I41" t="n">
-        <v>20.0</v>
+        <v>16.0</v>
       </c>
       <c r="J41" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="K41" t="b">
         <v>1</v>
@@ -1733,13 +1730,13 @@
         <v>51</v>
       </c>
       <c r="E42" t="n">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
       <c r="F42" t="n">
-        <v>171.0</v>
+        <v>162.0</v>
       </c>
       <c r="G42" t="n">
-        <v>27.0</v>
+        <v>23.0</v>
       </c>
       <c r="H42" t="b">
         <v>1</v>
@@ -1768,13 +1765,13 @@
         <v>52</v>
       </c>
       <c r="E43" t="n">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
       <c r="F43" t="n">
-        <v>171.0</v>
+        <v>162.0</v>
       </c>
       <c r="G43" t="n">
-        <v>27.0</v>
+        <v>23.0</v>
       </c>
       <c r="H43" t="b">
         <v>1</v>
@@ -1803,22 +1800,22 @@
         <v>53</v>
       </c>
       <c r="E44" t="n">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
       <c r="F44" t="n">
-        <v>171.0</v>
+        <v>162.0</v>
       </c>
       <c r="G44" t="n">
-        <v>27.0</v>
+        <v>23.0</v>
       </c>
       <c r="H44" t="b">
         <v>1</v>
       </c>
       <c r="I44" t="n">
-        <v>23.0</v>
+        <v>3.0</v>
       </c>
       <c r="J44" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="K44" t="b">
         <v>1</v>
@@ -1838,19 +1835,19 @@
         <v>54</v>
       </c>
       <c r="E45" t="n">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
       <c r="F45" t="n">
-        <v>171.0</v>
+        <v>162.0</v>
       </c>
       <c r="G45" t="n">
-        <v>27.0</v>
+        <v>23.0</v>
       </c>
       <c r="H45" t="b">
         <v>1</v>
       </c>
       <c r="I45" t="n">
-        <v>19.0</v>
+        <v>23.0</v>
       </c>
       <c r="J45" t="n">
         <v>4.0</v>
@@ -1873,22 +1870,22 @@
         <v>55</v>
       </c>
       <c r="E46" t="n">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
       <c r="F46" t="n">
-        <v>171.0</v>
+        <v>162.0</v>
       </c>
       <c r="G46" t="n">
-        <v>27.0</v>
+        <v>23.0</v>
       </c>
       <c r="H46" t="b">
         <v>1</v>
       </c>
       <c r="I46" t="n">
-        <v>6.0</v>
+        <v>24.0</v>
       </c>
       <c r="J46" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="K46" t="b">
         <v>1</v>
@@ -1908,22 +1905,22 @@
         <v>56</v>
       </c>
       <c r="E47" t="n">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
       <c r="F47" t="n">
-        <v>171.0</v>
+        <v>162.0</v>
       </c>
       <c r="G47" t="n">
-        <v>27.0</v>
+        <v>23.0</v>
       </c>
       <c r="H47" t="b">
         <v>1</v>
       </c>
       <c r="I47" t="n">
-        <v>10.0</v>
+        <v>3.0</v>
       </c>
       <c r="J47" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="K47" t="b">
         <v>1</v>
@@ -1943,19 +1940,19 @@
         <v>57</v>
       </c>
       <c r="E48" t="n">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
       <c r="F48" t="n">
-        <v>171.0</v>
+        <v>162.0</v>
       </c>
       <c r="G48" t="n">
-        <v>27.0</v>
+        <v>23.0</v>
       </c>
       <c r="H48" t="b">
         <v>1</v>
       </c>
       <c r="I48" t="n">
-        <v>3.0</v>
+        <v>8.0</v>
       </c>
       <c r="J48" t="n">
         <v>0.0</v>
@@ -1972,25 +1969,25 @@
         <v>20</v>
       </c>
       <c r="C49" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="D49" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E49" t="n">
-        <v>13.0</v>
+        <v>3.0</v>
       </c>
       <c r="F49" t="n">
-        <v>171.0</v>
+        <v>24.0</v>
       </c>
       <c r="G49" t="n">
-        <v>27.0</v>
+        <v>3.0</v>
       </c>
       <c r="H49" t="b">
         <v>1</v>
       </c>
       <c r="I49" t="n">
-        <v>8.0</v>
+        <v>4.0</v>
       </c>
       <c r="J49" t="n">
         <v>0.0</v>
@@ -2007,16 +2004,16 @@
         <v>20</v>
       </c>
       <c r="C50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D50" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="E50" t="n">
         <v>3.0</v>
       </c>
       <c r="F50" t="n">
-        <v>23.0</v>
+        <v>24.0</v>
       </c>
       <c r="G50" t="n">
         <v>3.0</v>
@@ -2025,7 +2022,7 @@
         <v>1</v>
       </c>
       <c r="I50" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="J50" t="n">
         <v>0.0</v>
@@ -2042,16 +2039,16 @@
         <v>20</v>
       </c>
       <c r="C51" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D51" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E51" t="n">
         <v>3.0</v>
       </c>
       <c r="F51" t="n">
-        <v>23.0</v>
+        <v>24.0</v>
       </c>
       <c r="G51" t="n">
         <v>3.0</v>
@@ -2060,10 +2057,10 @@
         <v>1</v>
       </c>
       <c r="I51" t="n">
-        <v>2.0</v>
+        <v>14.0</v>
       </c>
       <c r="J51" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="K51" t="b">
         <v>1</v>
@@ -2077,16 +2074,16 @@
         <v>20</v>
       </c>
       <c r="C52" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="D52" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="E52" t="n">
         <v>3.0</v>
       </c>
       <c r="F52" t="n">
-        <v>23.0</v>
+        <v>24.0</v>
       </c>
       <c r="G52" t="n">
         <v>3.0</v>
@@ -2095,10 +2092,10 @@
         <v>1</v>
       </c>
       <c r="I52" t="n">
-        <v>14.0</v>
+        <v>4.0</v>
       </c>
       <c r="J52" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="K52" t="b">
         <v>1</v>
@@ -2121,7 +2118,7 @@
         <v>3.0</v>
       </c>
       <c r="F53" t="n">
-        <v>23.0</v>
+        <v>24.0</v>
       </c>
       <c r="G53" t="n">
         <v>3.0</v>
@@ -2130,7 +2127,7 @@
         <v>1</v>
       </c>
       <c r="I53" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="J53" t="n">
         <v>0.0</v>
@@ -2150,13 +2147,13 @@
         <v>6</v>
       </c>
       <c r="D54" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="E54" t="n">
         <v>3.0</v>
       </c>
       <c r="F54" t="n">
-        <v>23.0</v>
+        <v>24.0</v>
       </c>
       <c r="G54" t="n">
         <v>3.0</v>
@@ -2165,10 +2162,10 @@
         <v>1</v>
       </c>
       <c r="I54" t="n">
-        <v>2.0</v>
+        <v>16.0</v>
       </c>
       <c r="J54" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="K54" t="b">
         <v>1</v>
@@ -2179,31 +2176,31 @@
         <v>54.0</v>
       </c>
       <c r="B55" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="C55" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="D55" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="E55" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="F55" t="n">
-        <v>23.0</v>
+        <v>31.0</v>
       </c>
       <c r="G55" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H55" t="b">
         <v>1</v>
       </c>
       <c r="I55" t="n">
-        <v>16.0</v>
+        <v>28.0</v>
       </c>
       <c r="J55" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="K55" t="b">
         <v>1</v>
@@ -2214,31 +2211,31 @@
         <v>55.0</v>
       </c>
       <c r="B56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C56" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D56" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E56" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="F56" t="n">
+        <v>53.0</v>
+      </c>
+      <c r="G56" t="n">
         <v>1.0</v>
       </c>
-      <c r="F56" t="n">
-        <v>31.0</v>
-      </c>
-      <c r="G56" t="n">
-        <v>2.0</v>
-      </c>
       <c r="H56" t="b">
         <v>1</v>
       </c>
       <c r="I56" t="n">
-        <v>28.0</v>
+        <v>3.0</v>
       </c>
       <c r="J56" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="K56" t="b">
         <v>1</v>
@@ -2249,10 +2246,10 @@
         <v>56.0</v>
       </c>
       <c r="B57" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C57" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D57" t="s">
         <v>67</v>
@@ -2284,10 +2281,10 @@
         <v>57.0</v>
       </c>
       <c r="B58" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C58" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D58" t="s">
         <v>68</v>
@@ -2319,10 +2316,10 @@
         <v>58.0</v>
       </c>
       <c r="B59" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C59" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D59" t="s">
         <v>69</v>
@@ -2354,10 +2351,10 @@
         <v>59.0</v>
       </c>
       <c r="B60" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C60" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D60" t="s">
         <v>70</v>
@@ -2389,10 +2386,10 @@
         <v>60.0</v>
       </c>
       <c r="B61" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C61" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D61" t="s">
         <v>71</v>
@@ -2410,10 +2407,10 @@
         <v>1</v>
       </c>
       <c r="I61" t="n">
-        <v>3.0</v>
+        <v>30.0</v>
       </c>
       <c r="J61" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="K61" t="b">
         <v>1</v>
@@ -2424,10 +2421,10 @@
         <v>61.0</v>
       </c>
       <c r="B62" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C62" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D62" t="s">
         <v>72</v>
@@ -2445,47 +2442,12 @@
         <v>1</v>
       </c>
       <c r="I62" t="n">
-        <v>30.0</v>
+        <v>4.0</v>
       </c>
       <c r="J62" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="K62" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="n">
-        <v>62.0</v>
-      </c>
-      <c r="B63" t="s">
-        <v>63</v>
-      </c>
-      <c r="C63" t="s">
-        <v>66</v>
-      </c>
-      <c r="D63" t="s">
-        <v>73</v>
-      </c>
-      <c r="E63" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="F63" t="n">
-        <v>53.0</v>
-      </c>
-      <c r="G63" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="H63" t="b">
-        <v>1</v>
-      </c>
-      <c r="I63" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="J63" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K63" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Avaliação e deteção de code smells
Precisa de melhorias

Co-Authored-By: dianamml17 <73841693+dianamml17@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ES-2Sem-2021-Grupo-5_metricas.xlsx
+++ b/ES-2Sem-2021-Grupo-5_metricas.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="136">
   <si>
     <t>MethodID</t>
   </si>
@@ -41,10 +41,10 @@
     <t>NOM_CLASS</t>
   </si>
   <si>
-    <t>sdfs</t>
-  </si>
-  <si>
-    <t>Custom_Rule</t>
+    <t>Is_God_Class</t>
+  </si>
+  <si>
+    <t>Is_Long_Method</t>
   </si>
   <si>
     <t>GUI</t>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>checkValidRule()</t>
+  </si>
+  <si>
+    <t>codeSmellsEvaluation(ArrayList&lt;String[]&gt; rulesResults, ArrayList&lt;String&gt; fileResults, int u, int i)</t>
   </si>
   <si>
     <t>enableDefaultValue(final JTextField tf, final String defaultValue)</t>
@@ -831,7 +834,7 @@
         <v>24</v>
       </c>
       <c r="E11" t="n">
-        <v>339.0</v>
+        <v>418.0</v>
       </c>
       <c r="F11" t="n">
         <v>3.0</v>
@@ -840,10 +843,10 @@
         <v>0.0</v>
       </c>
       <c r="H11" t="n">
-        <v>28.0</v>
+        <v>46.0</v>
       </c>
       <c r="I11" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="J11" t="b">
         <v>1</v>
@@ -866,7 +869,7 @@
         <v>25</v>
       </c>
       <c r="E12" t="n">
-        <v>339.0</v>
+        <v>418.0</v>
       </c>
       <c r="F12" t="n">
         <v>13.0</v>
@@ -875,10 +878,10 @@
         <v>1.0</v>
       </c>
       <c r="H12" t="n">
-        <v>28.0</v>
+        <v>46.0</v>
       </c>
       <c r="I12" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="J12" t="b">
         <v>1</v>
@@ -901,19 +904,19 @@
         <v>26</v>
       </c>
       <c r="E13" t="n">
-        <v>339.0</v>
+        <v>418.0</v>
       </c>
       <c r="F13" t="n">
-        <v>24.0</v>
+        <v>21.0</v>
       </c>
       <c r="G13" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="H13" t="n">
-        <v>28.0</v>
+        <v>46.0</v>
       </c>
       <c r="I13" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="J13" t="b">
         <v>1</v>
@@ -936,19 +939,19 @@
         <v>27</v>
       </c>
       <c r="E14" t="n">
-        <v>339.0</v>
+        <v>418.0</v>
       </c>
       <c r="F14" t="n">
-        <v>5.0</v>
+        <v>24.0</v>
       </c>
       <c r="G14" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="H14" t="n">
-        <v>28.0</v>
+        <v>46.0</v>
       </c>
       <c r="I14" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="J14" t="b">
         <v>1</v>
@@ -971,25 +974,25 @@
         <v>28</v>
       </c>
       <c r="E15" t="n">
-        <v>339.0</v>
+        <v>418.0</v>
       </c>
       <c r="F15" t="n">
-        <v>8.0</v>
+        <v>5.0</v>
       </c>
       <c r="G15" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H15" t="n">
-        <v>28.0</v>
+        <v>46.0</v>
       </c>
       <c r="I15" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="J15" t="b">
         <v>1</v>
       </c>
-      <c r="K15" t="s">
-        <v>14</v>
+      <c r="K15" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -1006,25 +1009,25 @@
         <v>29</v>
       </c>
       <c r="E16" t="n">
-        <v>339.0</v>
+        <v>418.0</v>
       </c>
       <c r="F16" t="n">
-        <v>19.0</v>
+        <v>8.0</v>
       </c>
       <c r="G16" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="H16" t="n">
-        <v>28.0</v>
+        <v>46.0</v>
       </c>
       <c r="I16" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="J16" t="b">
         <v>1</v>
       </c>
-      <c r="K16" t="b">
-        <v>1</v>
+      <c r="K16" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="17">
@@ -1041,19 +1044,19 @@
         <v>30</v>
       </c>
       <c r="E17" t="n">
-        <v>339.0</v>
+        <v>418.0</v>
       </c>
       <c r="F17" t="n">
-        <v>219.0</v>
+        <v>19.0</v>
       </c>
       <c r="G17" t="n">
-        <v>18.0</v>
+        <v>4.0</v>
       </c>
       <c r="H17" t="n">
-        <v>28.0</v>
+        <v>46.0</v>
       </c>
       <c r="I17" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="J17" t="b">
         <v>1</v>
@@ -1076,25 +1079,25 @@
         <v>31</v>
       </c>
       <c r="E18" t="n">
-        <v>339.0</v>
+        <v>418.0</v>
       </c>
       <c r="F18" t="n">
-        <v>12.0</v>
+        <v>210.0</v>
       </c>
       <c r="G18" t="n">
-        <v>0.0</v>
+        <v>18.0</v>
       </c>
       <c r="H18" t="n">
-        <v>28.0</v>
+        <v>46.0</v>
       </c>
       <c r="I18" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="J18" t="b">
         <v>1</v>
       </c>
-      <c r="K18" t="s">
-        <v>14</v>
+      <c r="K18" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -1111,25 +1114,25 @@
         <v>32</v>
       </c>
       <c r="E19" t="n">
-        <v>339.0</v>
+        <v>418.0</v>
       </c>
       <c r="F19" t="n">
-        <v>14.0</v>
+        <v>12.0</v>
       </c>
       <c r="G19" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H19" t="n">
-        <v>28.0</v>
+        <v>46.0</v>
       </c>
       <c r="I19" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="J19" t="b">
         <v>1</v>
       </c>
-      <c r="K19" t="b">
-        <v>1</v>
+      <c r="K19" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="20">
@@ -1146,19 +1149,19 @@
         <v>33</v>
       </c>
       <c r="E20" t="n">
-        <v>339.0</v>
+        <v>418.0</v>
       </c>
       <c r="F20" t="n">
-        <v>41.0</v>
+        <v>14.0</v>
       </c>
       <c r="G20" t="n">
         <v>1.0</v>
       </c>
       <c r="H20" t="n">
-        <v>28.0</v>
+        <v>46.0</v>
       </c>
       <c r="I20" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="J20" t="b">
         <v>1</v>
@@ -1175,22 +1178,22 @@
         <v>11</v>
       </c>
       <c r="C21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" t="s">
         <v>34</v>
       </c>
-      <c r="D21" t="s">
-        <v>35</v>
-      </c>
       <c r="E21" t="n">
-        <v>139.0</v>
+        <v>418.0</v>
       </c>
       <c r="F21" t="n">
-        <v>2.0</v>
+        <v>100.0</v>
       </c>
       <c r="G21" t="n">
-        <v>0.0</v>
+        <v>13.0</v>
       </c>
       <c r="H21" t="n">
-        <v>6.0</v>
+        <v>46.0</v>
       </c>
       <c r="I21" t="n">
         <v>11.0</v>
@@ -1198,8 +1201,8 @@
       <c r="J21" t="b">
         <v>1</v>
       </c>
-      <c r="K21" t="s">
-        <v>14</v>
+      <c r="K21" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -1210,7 +1213,7 @@
         <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D22" t="s">
         <v>36</v>
@@ -1219,10 +1222,10 @@
         <v>139.0</v>
       </c>
       <c r="F22" t="n">
-        <v>42.0</v>
+        <v>2.0</v>
       </c>
       <c r="G22" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H22" t="n">
         <v>6.0</v>
@@ -1233,8 +1236,8 @@
       <c r="J22" t="b">
         <v>1</v>
       </c>
-      <c r="K22" t="b">
-        <v>1</v>
+      <c r="K22" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="23">
@@ -1245,7 +1248,7 @@
         <v>11</v>
       </c>
       <c r="C23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D23" t="s">
         <v>37</v>
@@ -1254,10 +1257,10 @@
         <v>139.0</v>
       </c>
       <c r="F23" t="n">
-        <v>3.0</v>
+        <v>42.0</v>
       </c>
       <c r="G23" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H23" t="n">
         <v>6.0</v>
@@ -1268,8 +1271,8 @@
       <c r="J23" t="b">
         <v>1</v>
       </c>
-      <c r="K23" t="s">
-        <v>14</v>
+      <c r="K23" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="24">
@@ -1280,7 +1283,7 @@
         <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D24" t="s">
         <v>38</v>
@@ -1315,7 +1318,7 @@
         <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D25" t="s">
         <v>39</v>
@@ -1324,7 +1327,7 @@
         <v>139.0</v>
       </c>
       <c r="F25" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="G25" t="n">
         <v>0.0</v>
@@ -1350,7 +1353,7 @@
         <v>11</v>
       </c>
       <c r="C26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D26" t="s">
         <v>40</v>
@@ -1359,10 +1362,10 @@
         <v>139.0</v>
       </c>
       <c r="F26" t="n">
-        <v>19.0</v>
+        <v>5.0</v>
       </c>
       <c r="G26" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="H26" t="n">
         <v>6.0</v>
@@ -1373,8 +1376,8 @@
       <c r="J26" t="b">
         <v>1</v>
       </c>
-      <c r="K26" t="b">
-        <v>1</v>
+      <c r="K26" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="27">
@@ -1385,7 +1388,7 @@
         <v>11</v>
       </c>
       <c r="C27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D27" t="s">
         <v>41</v>
@@ -1394,10 +1397,10 @@
         <v>139.0</v>
       </c>
       <c r="F27" t="n">
-        <v>3.0</v>
+        <v>19.0</v>
       </c>
       <c r="G27" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="H27" t="n">
         <v>6.0</v>
@@ -1408,8 +1411,8 @@
       <c r="J27" t="b">
         <v>1</v>
       </c>
-      <c r="K27" t="s">
-        <v>14</v>
+      <c r="K27" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -1420,7 +1423,7 @@
         <v>11</v>
       </c>
       <c r="C28" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D28" t="s">
         <v>42</v>
@@ -1455,7 +1458,7 @@
         <v>11</v>
       </c>
       <c r="C29" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D29" t="s">
         <v>43</v>
@@ -1490,19 +1493,19 @@
         <v>11</v>
       </c>
       <c r="C30" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D30" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="E30" t="n">
         <v>139.0</v>
       </c>
       <c r="F30" t="n">
-        <v>19.0</v>
+        <v>3.0</v>
       </c>
       <c r="G30" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="H30" t="n">
         <v>6.0</v>
@@ -1513,8 +1516,8 @@
       <c r="J30" t="b">
         <v>1</v>
       </c>
-      <c r="K30" t="b">
-        <v>1</v>
+      <c r="K30" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="31">
@@ -1525,19 +1528,19 @@
         <v>11</v>
       </c>
       <c r="C31" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D31" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="E31" t="n">
         <v>139.0</v>
       </c>
       <c r="F31" t="n">
-        <v>3.0</v>
+        <v>19.0</v>
       </c>
       <c r="G31" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H31" t="n">
         <v>6.0</v>
@@ -1548,8 +1551,8 @@
       <c r="J31" t="b">
         <v>1</v>
       </c>
-      <c r="K31" t="s">
-        <v>14</v>
+      <c r="K31" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -1560,13 +1563,13 @@
         <v>11</v>
       </c>
       <c r="C32" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" t="s">
         <v>45</v>
       </c>
-      <c r="D32" t="s">
-        <v>46</v>
-      </c>
       <c r="E32" t="n">
-        <v>69.0</v>
+        <v>139.0</v>
       </c>
       <c r="F32" t="n">
         <v>3.0</v>
@@ -1575,10 +1578,10 @@
         <v>0.0</v>
       </c>
       <c r="H32" t="n">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="I32" t="n">
-        <v>7.0</v>
+        <v>11.0</v>
       </c>
       <c r="J32" t="b">
         <v>1</v>
@@ -1595,7 +1598,7 @@
         <v>11</v>
       </c>
       <c r="C33" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D33" t="s">
         <v>47</v>
@@ -1630,7 +1633,7 @@
         <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D34" t="s">
         <v>48</v>
@@ -1665,7 +1668,7 @@
         <v>11</v>
       </c>
       <c r="C35" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D35" t="s">
         <v>49</v>
@@ -1674,10 +1677,10 @@
         <v>69.0</v>
       </c>
       <c r="F35" t="n">
-        <v>7.0</v>
+        <v>3.0</v>
       </c>
       <c r="G35" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H35" t="n">
         <v>7.0</v>
@@ -1688,8 +1691,8 @@
       <c r="J35" t="b">
         <v>1</v>
       </c>
-      <c r="K35" t="b">
-        <v>1</v>
+      <c r="K35" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="36">
@@ -1700,7 +1703,7 @@
         <v>11</v>
       </c>
       <c r="C36" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D36" t="s">
         <v>50</v>
@@ -1709,10 +1712,10 @@
         <v>69.0</v>
       </c>
       <c r="F36" t="n">
-        <v>40.0</v>
+        <v>7.0</v>
       </c>
       <c r="G36" t="n">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
       <c r="H36" t="n">
         <v>7.0</v>
@@ -1735,7 +1738,7 @@
         <v>11</v>
       </c>
       <c r="C37" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D37" t="s">
         <v>51</v>
@@ -1744,10 +1747,10 @@
         <v>69.0</v>
       </c>
       <c r="F37" t="n">
-        <v>5.0</v>
+        <v>40.0</v>
       </c>
       <c r="G37" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
       <c r="H37" t="n">
         <v>7.0</v>
@@ -1758,8 +1761,8 @@
       <c r="J37" t="b">
         <v>1</v>
       </c>
-      <c r="K37" t="s">
-        <v>14</v>
+      <c r="K37" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -1770,7 +1773,7 @@
         <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D38" t="s">
         <v>52</v>
@@ -1779,7 +1782,7 @@
         <v>69.0</v>
       </c>
       <c r="F38" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="G38" t="n">
         <v>0.0</v>
@@ -1802,28 +1805,28 @@
         <v>38.0</v>
       </c>
       <c r="B39" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" t="s">
         <v>53</v>
       </c>
-      <c r="C39" t="s">
-        <v>54</v>
-      </c>
-      <c r="D39" t="s">
-        <v>55</v>
-      </c>
       <c r="E39" t="n">
-        <v>35.0</v>
+        <v>69.0</v>
       </c>
       <c r="F39" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="G39" t="n">
         <v>0.0</v>
       </c>
       <c r="H39" t="n">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="I39" t="n">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="J39" t="b">
         <v>1</v>
@@ -1837,10 +1840,10 @@
         <v>39.0</v>
       </c>
       <c r="B40" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C40" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D40" t="s">
         <v>56</v>
@@ -1849,10 +1852,10 @@
         <v>35.0</v>
       </c>
       <c r="F40" t="n">
-        <v>17.0</v>
+        <v>5.0</v>
       </c>
       <c r="G40" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="H40" t="n">
         <v>5.0</v>
@@ -1863,8 +1866,8 @@
       <c r="J40" t="b">
         <v>1</v>
       </c>
-      <c r="K40" t="b">
-        <v>1</v>
+      <c r="K40" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="41">
@@ -1872,10 +1875,10 @@
         <v>40.0</v>
       </c>
       <c r="B41" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C41" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D41" t="s">
         <v>57</v>
@@ -1884,10 +1887,10 @@
         <v>35.0</v>
       </c>
       <c r="F41" t="n">
-        <v>8.0</v>
+        <v>17.0</v>
       </c>
       <c r="G41" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="H41" t="n">
         <v>5.0</v>
@@ -1907,34 +1910,34 @@
         <v>41.0</v>
       </c>
       <c r="B42" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C42" t="s">
+        <v>55</v>
+      </c>
+      <c r="D42" t="s">
         <v>58</v>
       </c>
-      <c r="D42" t="s">
-        <v>59</v>
-      </c>
       <c r="E42" t="n">
-        <v>38.0</v>
+        <v>35.0</v>
       </c>
       <c r="F42" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="G42" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H42" t="n">
         <v>5.0</v>
       </c>
-      <c r="G42" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H42" t="n">
-        <v>4.0</v>
-      </c>
       <c r="I42" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="J42" t="b">
         <v>1</v>
       </c>
-      <c r="K42" t="s">
-        <v>14</v>
+      <c r="K42" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="43">
@@ -1942,13 +1945,13 @@
         <v>42.0</v>
       </c>
       <c r="B43" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C43" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D43" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="E43" t="n">
         <v>38.0</v>
@@ -1957,7 +1960,7 @@
         <v>5.0</v>
       </c>
       <c r="G43" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H43" t="n">
         <v>4.0</v>
@@ -1968,8 +1971,8 @@
       <c r="J43" t="b">
         <v>1</v>
       </c>
-      <c r="K43" t="b">
-        <v>1</v>
+      <c r="K43" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="44">
@@ -1977,10 +1980,10 @@
         <v>43.0</v>
       </c>
       <c r="B44" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C44" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D44" t="s">
         <v>57</v>
@@ -1989,7 +1992,7 @@
         <v>38.0</v>
       </c>
       <c r="F44" t="n">
-        <v>9.0</v>
+        <v>5.0</v>
       </c>
       <c r="G44" t="n">
         <v>1.0</v>
@@ -2012,22 +2015,22 @@
         <v>44.0</v>
       </c>
       <c r="B45" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C45" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45" t="s">
         <v>58</v>
-      </c>
-      <c r="D45" t="s">
-        <v>60</v>
       </c>
       <c r="E45" t="n">
         <v>38.0</v>
       </c>
       <c r="F45" t="n">
-        <v>14.0</v>
+        <v>9.0</v>
       </c>
       <c r="G45" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="H45" t="n">
         <v>4.0</v>
@@ -2047,34 +2050,34 @@
         <v>45.0</v>
       </c>
       <c r="B46" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C46" t="s">
+        <v>59</v>
+      </c>
+      <c r="D46" t="s">
         <v>61</v>
       </c>
-      <c r="D46" t="s">
-        <v>62</v>
-      </c>
       <c r="E46" t="n">
-        <v>25.0</v>
+        <v>38.0</v>
       </c>
       <c r="F46" t="n">
-        <v>5.0</v>
+        <v>14.0</v>
       </c>
       <c r="G46" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H46" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="I46" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="J46" t="b">
         <v>1</v>
       </c>
-      <c r="K46" t="s">
-        <v>14</v>
+      <c r="K46" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="47">
@@ -2082,22 +2085,22 @@
         <v>46.0</v>
       </c>
       <c r="B47" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C47" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D47" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="E47" t="n">
         <v>25.0</v>
       </c>
       <c r="F47" t="n">
-        <v>8.0</v>
+        <v>5.0</v>
       </c>
       <c r="G47" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H47" t="n">
         <v>2.0</v>
@@ -2108,8 +2111,8 @@
       <c r="J47" t="b">
         <v>1</v>
       </c>
-      <c r="K47" t="b">
-        <v>1</v>
+      <c r="K47" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="48">
@@ -2117,10 +2120,10 @@
         <v>47.0</v>
       </c>
       <c r="B48" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C48" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D48" t="s">
         <v>57</v>
@@ -2152,34 +2155,34 @@
         <v>48.0</v>
       </c>
       <c r="B49" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C49" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D49" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E49" t="n">
-        <v>203.0</v>
+        <v>25.0</v>
       </c>
       <c r="F49" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="G49" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H49" t="n">
         <v>2.0</v>
       </c>
-      <c r="G49" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H49" t="n">
-        <v>18.0</v>
-      </c>
       <c r="I49" t="n">
-        <v>20.0</v>
+        <v>3.0</v>
       </c>
       <c r="J49" t="b">
         <v>1</v>
       </c>
-      <c r="K49" t="s">
-        <v>14</v>
+      <c r="K49" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="50">
@@ -2187,10 +2190,10 @@
         <v>49.0</v>
       </c>
       <c r="B50" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C50" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D50" t="s">
         <v>65</v>
@@ -2199,7 +2202,7 @@
         <v>203.0</v>
       </c>
       <c r="F50" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c r="G50" t="n">
         <v>0.0</v>
@@ -2222,10 +2225,10 @@
         <v>50.0</v>
       </c>
       <c r="B51" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C51" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D51" t="s">
         <v>66</v>
@@ -2234,7 +2237,7 @@
         <v>203.0</v>
       </c>
       <c r="F51" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="G51" t="n">
         <v>0.0</v>
@@ -2257,10 +2260,10 @@
         <v>51.0</v>
       </c>
       <c r="B52" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D52" t="s">
         <v>67</v>
@@ -2292,10 +2295,10 @@
         <v>52.0</v>
       </c>
       <c r="B53" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C53" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D53" t="s">
         <v>68</v>
@@ -2304,10 +2307,10 @@
         <v>203.0</v>
       </c>
       <c r="F53" t="n">
-        <v>23.0</v>
+        <v>3.0</v>
       </c>
       <c r="G53" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="H53" t="n">
         <v>18.0</v>
@@ -2318,8 +2321,8 @@
       <c r="J53" t="b">
         <v>1</v>
       </c>
-      <c r="K53" t="b">
-        <v>1</v>
+      <c r="K53" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="54">
@@ -2327,10 +2330,10 @@
         <v>53.0</v>
       </c>
       <c r="B54" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C54" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D54" t="s">
         <v>69</v>
@@ -2339,10 +2342,10 @@
         <v>203.0</v>
       </c>
       <c r="F54" t="n">
-        <v>13.0</v>
+        <v>23.0</v>
       </c>
       <c r="G54" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H54" t="n">
         <v>18.0</v>
@@ -2362,10 +2365,10 @@
         <v>54.0</v>
       </c>
       <c r="B55" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C55" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D55" t="s">
         <v>70</v>
@@ -2374,10 +2377,10 @@
         <v>203.0</v>
       </c>
       <c r="F55" t="n">
-        <v>41.0</v>
+        <v>13.0</v>
       </c>
       <c r="G55" t="n">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
       <c r="H55" t="n">
         <v>18.0</v>
@@ -2397,10 +2400,10 @@
         <v>55.0</v>
       </c>
       <c r="B56" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D56" t="s">
         <v>71</v>
@@ -2409,10 +2412,10 @@
         <v>203.0</v>
       </c>
       <c r="F56" t="n">
-        <v>3.0</v>
+        <v>41.0</v>
       </c>
       <c r="G56" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
       <c r="H56" t="n">
         <v>18.0</v>
@@ -2423,8 +2426,8 @@
       <c r="J56" t="b">
         <v>1</v>
       </c>
-      <c r="K56" t="s">
-        <v>14</v>
+      <c r="K56" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="57">
@@ -2432,10 +2435,10 @@
         <v>56.0</v>
       </c>
       <c r="B57" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C57" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D57" t="s">
         <v>72</v>
@@ -2467,10 +2470,10 @@
         <v>57.0</v>
       </c>
       <c r="B58" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C58" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D58" t="s">
         <v>73</v>
@@ -2502,10 +2505,10 @@
         <v>58.0</v>
       </c>
       <c r="B59" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C59" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D59" t="s">
         <v>74</v>
@@ -2537,10 +2540,10 @@
         <v>59.0</v>
       </c>
       <c r="B60" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C60" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D60" t="s">
         <v>75</v>
@@ -2572,10 +2575,10 @@
         <v>60.0</v>
       </c>
       <c r="B61" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C61" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D61" t="s">
         <v>76</v>
@@ -2607,10 +2610,10 @@
         <v>61.0</v>
       </c>
       <c r="B62" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C62" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D62" t="s">
         <v>77</v>
@@ -2642,10 +2645,10 @@
         <v>62.0</v>
       </c>
       <c r="B63" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C63" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D63" t="s">
         <v>78</v>
@@ -2677,10 +2680,10 @@
         <v>63.0</v>
       </c>
       <c r="B64" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C64" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D64" t="s">
         <v>79</v>
@@ -2689,10 +2692,10 @@
         <v>203.0</v>
       </c>
       <c r="F64" t="n">
-        <v>13.0</v>
+        <v>3.0</v>
       </c>
       <c r="G64" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="H64" t="n">
         <v>18.0</v>
@@ -2703,8 +2706,8 @@
       <c r="J64" t="b">
         <v>1</v>
       </c>
-      <c r="K64" t="b">
-        <v>1</v>
+      <c r="K64" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="65">
@@ -2712,10 +2715,10 @@
         <v>64.0</v>
       </c>
       <c r="B65" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C65" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D65" t="s">
         <v>80</v>
@@ -2724,10 +2727,10 @@
         <v>203.0</v>
       </c>
       <c r="F65" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="G65" t="n">
         <v>4.0</v>
-      </c>
-      <c r="G65" t="n">
-        <v>0.0</v>
       </c>
       <c r="H65" t="n">
         <v>18.0</v>
@@ -2738,8 +2741,8 @@
       <c r="J65" t="b">
         <v>1</v>
       </c>
-      <c r="K65" t="s">
-        <v>14</v>
+      <c r="K65" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="66">
@@ -2747,10 +2750,10 @@
         <v>65.0</v>
       </c>
       <c r="B66" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C66" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D66" t="s">
         <v>81</v>
@@ -2759,7 +2762,7 @@
         <v>203.0</v>
       </c>
       <c r="F66" t="n">
-        <v>42.0</v>
+        <v>4.0</v>
       </c>
       <c r="G66" t="n">
         <v>0.0</v>
@@ -2782,10 +2785,10 @@
         <v>66.0</v>
       </c>
       <c r="B67" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C67" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D67" t="s">
         <v>82</v>
@@ -2794,7 +2797,7 @@
         <v>203.0</v>
       </c>
       <c r="F67" t="n">
-        <v>4.0</v>
+        <v>42.0</v>
       </c>
       <c r="G67" t="n">
         <v>0.0</v>
@@ -2817,10 +2820,10 @@
         <v>67.0</v>
       </c>
       <c r="B68" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C68" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D68" t="s">
         <v>83</v>
@@ -2829,10 +2832,10 @@
         <v>203.0</v>
       </c>
       <c r="F68" t="n">
-        <v>27.0</v>
+        <v>4.0</v>
       </c>
       <c r="G68" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="H68" t="n">
         <v>18.0</v>
@@ -2843,8 +2846,8 @@
       <c r="J68" t="b">
         <v>1</v>
       </c>
-      <c r="K68" t="b">
-        <v>1</v>
+      <c r="K68" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="69">
@@ -2852,34 +2855,34 @@
         <v>68.0</v>
       </c>
       <c r="B69" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C69" t="s">
+        <v>64</v>
+      </c>
+      <c r="D69" t="s">
         <v>84</v>
       </c>
-      <c r="D69" t="s">
-        <v>85</v>
-      </c>
       <c r="E69" t="n">
-        <v>167.0</v>
+        <v>203.0</v>
       </c>
       <c r="F69" t="n">
-        <v>6.0</v>
+        <v>27.0</v>
       </c>
       <c r="G69" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="H69" t="n">
-        <v>23.0</v>
+        <v>18.0</v>
       </c>
       <c r="I69" t="n">
-        <v>13.0</v>
+        <v>20.0</v>
       </c>
       <c r="J69" t="b">
         <v>1</v>
       </c>
-      <c r="K69" t="s">
-        <v>14</v>
+      <c r="K69" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="70">
@@ -2887,22 +2890,22 @@
         <v>69.0</v>
       </c>
       <c r="B70" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C70" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D70" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="E70" t="n">
         <v>167.0</v>
       </c>
       <c r="F70" t="n">
-        <v>37.0</v>
+        <v>6.0</v>
       </c>
       <c r="G70" t="n">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
       <c r="H70" t="n">
         <v>23.0</v>
@@ -2913,8 +2916,8 @@
       <c r="J70" t="b">
         <v>1</v>
       </c>
-      <c r="K70" t="b">
-        <v>1</v>
+      <c r="K70" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="71">
@@ -2922,22 +2925,22 @@
         <v>70.0</v>
       </c>
       <c r="B71" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C71" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D71" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="E71" t="n">
         <v>167.0</v>
       </c>
       <c r="F71" t="n">
-        <v>21.0</v>
+        <v>37.0</v>
       </c>
       <c r="G71" t="n">
-        <v>5.0</v>
+        <v>8.0</v>
       </c>
       <c r="H71" t="n">
         <v>23.0</v>
@@ -2957,10 +2960,10 @@
         <v>71.0</v>
       </c>
       <c r="B72" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C72" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D72" t="s">
         <v>87</v>
@@ -2969,10 +2972,10 @@
         <v>167.0</v>
       </c>
       <c r="F72" t="n">
-        <v>3.0</v>
+        <v>21.0</v>
       </c>
       <c r="G72" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="H72" t="n">
         <v>23.0</v>
@@ -2983,8 +2986,8 @@
       <c r="J72" t="b">
         <v>1</v>
       </c>
-      <c r="K72" t="s">
-        <v>14</v>
+      <c r="K72" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="73">
@@ -2992,10 +2995,10 @@
         <v>72.0</v>
       </c>
       <c r="B73" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C73" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D73" t="s">
         <v>88</v>
@@ -3004,10 +3007,10 @@
         <v>167.0</v>
       </c>
       <c r="F73" t="n">
-        <v>16.0</v>
+        <v>3.0</v>
       </c>
       <c r="G73" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="H73" t="n">
         <v>23.0</v>
@@ -3018,8 +3021,8 @@
       <c r="J73" t="b">
         <v>1</v>
       </c>
-      <c r="K73" t="b">
-        <v>1</v>
+      <c r="K73" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="74">
@@ -3027,10 +3030,10 @@
         <v>73.0</v>
       </c>
       <c r="B74" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C74" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D74" t="s">
         <v>89</v>
@@ -3039,10 +3042,10 @@
         <v>167.0</v>
       </c>
       <c r="F74" t="n">
-        <v>3.0</v>
+        <v>16.0</v>
       </c>
       <c r="G74" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H74" t="n">
         <v>23.0</v>
@@ -3053,8 +3056,8 @@
       <c r="J74" t="b">
         <v>1</v>
       </c>
-      <c r="K74" t="s">
-        <v>14</v>
+      <c r="K74" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="75">
@@ -3062,10 +3065,10 @@
         <v>74.0</v>
       </c>
       <c r="B75" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C75" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D75" t="s">
         <v>90</v>
@@ -3097,10 +3100,10 @@
         <v>75.0</v>
       </c>
       <c r="B76" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C76" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D76" t="s">
         <v>91</v>
@@ -3132,10 +3135,10 @@
         <v>76.0</v>
       </c>
       <c r="B77" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C77" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D77" t="s">
         <v>92</v>
@@ -3144,10 +3147,10 @@
         <v>167.0</v>
       </c>
       <c r="F77" t="n">
-        <v>23.0</v>
+        <v>3.0</v>
       </c>
       <c r="G77" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="H77" t="n">
         <v>23.0</v>
@@ -3158,8 +3161,8 @@
       <c r="J77" t="b">
         <v>1</v>
       </c>
-      <c r="K77" t="b">
-        <v>1</v>
+      <c r="K77" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="78">
@@ -3167,10 +3170,10 @@
         <v>77.0</v>
       </c>
       <c r="B78" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C78" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D78" t="s">
         <v>93</v>
@@ -3179,7 +3182,7 @@
         <v>167.0</v>
       </c>
       <c r="F78" t="n">
-        <v>24.0</v>
+        <v>23.0</v>
       </c>
       <c r="G78" t="n">
         <v>4.0</v>
@@ -3202,10 +3205,10 @@
         <v>78.0</v>
       </c>
       <c r="B79" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C79" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D79" t="s">
         <v>94</v>
@@ -3214,10 +3217,10 @@
         <v>167.0</v>
       </c>
       <c r="F79" t="n">
-        <v>3.0</v>
+        <v>24.0</v>
       </c>
       <c r="G79" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="H79" t="n">
         <v>23.0</v>
@@ -3228,8 +3231,8 @@
       <c r="J79" t="b">
         <v>1</v>
       </c>
-      <c r="K79" t="s">
-        <v>14</v>
+      <c r="K79" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="80">
@@ -3237,10 +3240,10 @@
         <v>79.0</v>
       </c>
       <c r="B80" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C80" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D80" t="s">
         <v>95</v>
@@ -3272,10 +3275,10 @@
         <v>80.0</v>
       </c>
       <c r="B81" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C81" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D81" t="s">
         <v>96</v>
@@ -3284,7 +3287,7 @@
         <v>167.0</v>
       </c>
       <c r="F81" t="n">
-        <v>8.0</v>
+        <v>3.0</v>
       </c>
       <c r="G81" t="n">
         <v>0.0</v>
@@ -3307,28 +3310,28 @@
         <v>81.0</v>
       </c>
       <c r="B82" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C82" t="s">
+        <v>85</v>
+      </c>
+      <c r="D82" t="s">
         <v>97</v>
       </c>
-      <c r="D82" t="s">
-        <v>98</v>
-      </c>
       <c r="E82" t="n">
-        <v>25.0</v>
+        <v>167.0</v>
       </c>
       <c r="F82" t="n">
-        <v>5.0</v>
+        <v>8.0</v>
       </c>
       <c r="G82" t="n">
         <v>0.0</v>
       </c>
       <c r="H82" t="n">
-        <v>3.0</v>
+        <v>23.0</v>
       </c>
       <c r="I82" t="n">
-        <v>3.0</v>
+        <v>13.0</v>
       </c>
       <c r="J82" t="b">
         <v>1</v>
@@ -3342,19 +3345,19 @@
         <v>82.0</v>
       </c>
       <c r="B83" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C83" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D83" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="E83" t="n">
         <v>25.0</v>
       </c>
       <c r="F83" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="G83" t="n">
         <v>0.0</v>
@@ -3377,10 +3380,10 @@
         <v>83.0</v>
       </c>
       <c r="B84" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C84" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D84" t="s">
         <v>57</v>
@@ -3389,10 +3392,10 @@
         <v>25.0</v>
       </c>
       <c r="F84" t="n">
-        <v>14.0</v>
+        <v>2.0</v>
       </c>
       <c r="G84" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="H84" t="n">
         <v>3.0</v>
@@ -3403,8 +3406,8 @@
       <c r="J84" t="b">
         <v>1</v>
       </c>
-      <c r="K84" t="b">
-        <v>1</v>
+      <c r="K84" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="85">
@@ -3412,22 +3415,22 @@
         <v>84.0</v>
       </c>
       <c r="B85" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C85" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D85" t="s">
-        <v>100</v>
+        <v>58</v>
       </c>
       <c r="E85" t="n">
         <v>25.0</v>
       </c>
       <c r="F85" t="n">
-        <v>5.0</v>
+        <v>14.0</v>
       </c>
       <c r="G85" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="H85" t="n">
         <v>3.0</v>
@@ -3438,8 +3441,8 @@
       <c r="J85" t="b">
         <v>1</v>
       </c>
-      <c r="K85" t="s">
-        <v>14</v>
+      <c r="K85" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="86">
@@ -3447,19 +3450,19 @@
         <v>85.0</v>
       </c>
       <c r="B86" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C86" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D86" t="s">
-        <v>56</v>
+        <v>101</v>
       </c>
       <c r="E86" t="n">
         <v>25.0</v>
       </c>
       <c r="F86" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="G86" t="n">
         <v>0.0</v>
@@ -3482,10 +3485,10 @@
         <v>86.0</v>
       </c>
       <c r="B87" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C87" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D87" t="s">
         <v>57</v>
@@ -3494,10 +3497,10 @@
         <v>25.0</v>
       </c>
       <c r="F87" t="n">
-        <v>16.0</v>
+        <v>2.0</v>
       </c>
       <c r="G87" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="H87" t="n">
         <v>3.0</v>
@@ -3508,8 +3511,8 @@
       <c r="J87" t="b">
         <v>1</v>
       </c>
-      <c r="K87" t="b">
-        <v>1</v>
+      <c r="K87" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="88">
@@ -3517,28 +3520,28 @@
         <v>87.0</v>
       </c>
       <c r="B88" t="s">
-        <v>101</v>
+        <v>54</v>
       </c>
       <c r="C88" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D88" t="s">
-        <v>103</v>
+        <v>58</v>
       </c>
       <c r="E88" t="n">
-        <v>42.0</v>
+        <v>25.0</v>
       </c>
       <c r="F88" t="n">
-        <v>9.0</v>
+        <v>16.0</v>
       </c>
       <c r="G88" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H88" t="n">
         <v>3.0</v>
       </c>
       <c r="I88" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="J88" t="b">
         <v>1</v>
@@ -3552,10 +3555,10 @@
         <v>88.0</v>
       </c>
       <c r="B89" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C89" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D89" t="s">
         <v>104</v>
@@ -3564,10 +3567,10 @@
         <v>42.0</v>
       </c>
       <c r="F89" t="n">
-        <v>29.0</v>
+        <v>9.0</v>
       </c>
       <c r="G89" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="H89" t="n">
         <v>3.0</v>
@@ -3587,34 +3590,34 @@
         <v>89.0</v>
       </c>
       <c r="B90" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C90" t="s">
+        <v>103</v>
+      </c>
+      <c r="D90" t="s">
         <v>105</v>
       </c>
-      <c r="D90" t="s">
-        <v>106</v>
-      </c>
       <c r="E90" t="n">
-        <v>105.0</v>
+        <v>42.0</v>
       </c>
       <c r="F90" t="n">
-        <v>3.0</v>
+        <v>29.0</v>
       </c>
       <c r="G90" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H90" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="I90" t="n">
-        <v>12.0</v>
+        <v>2.0</v>
       </c>
       <c r="J90" t="b">
         <v>1</v>
       </c>
-      <c r="K90" t="s">
-        <v>14</v>
+      <c r="K90" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="91">
@@ -3622,10 +3625,10 @@
         <v>90.0</v>
       </c>
       <c r="B91" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C91" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D91" t="s">
         <v>107</v>
@@ -3634,7 +3637,7 @@
         <v>105.0</v>
       </c>
       <c r="F91" t="n">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="G91" t="n">
         <v>0.0</v>
@@ -3657,10 +3660,10 @@
         <v>91.0</v>
       </c>
       <c r="B92" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C92" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D92" t="s">
         <v>108</v>
@@ -3669,7 +3672,7 @@
         <v>105.0</v>
       </c>
       <c r="F92" t="n">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="G92" t="n">
         <v>0.0</v>
@@ -3692,10 +3695,10 @@
         <v>92.0</v>
       </c>
       <c r="B93" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C93" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D93" t="s">
         <v>109</v>
@@ -3704,7 +3707,7 @@
         <v>105.0</v>
       </c>
       <c r="F93" t="n">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="G93" t="n">
         <v>0.0</v>
@@ -3727,10 +3730,10 @@
         <v>93.0</v>
       </c>
       <c r="B94" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C94" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D94" t="s">
         <v>110</v>
@@ -3762,10 +3765,10 @@
         <v>94.0</v>
       </c>
       <c r="B95" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C95" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D95" t="s">
         <v>111</v>
@@ -3797,10 +3800,10 @@
         <v>95.0</v>
       </c>
       <c r="B96" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C96" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D96" t="s">
         <v>112</v>
@@ -3832,10 +3835,10 @@
         <v>96.0</v>
       </c>
       <c r="B97" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C97" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D97" t="s">
         <v>113</v>
@@ -3844,7 +3847,7 @@
         <v>105.0</v>
       </c>
       <c r="F97" t="n">
-        <v>8.0</v>
+        <v>3.0</v>
       </c>
       <c r="G97" t="n">
         <v>0.0</v>
@@ -3867,10 +3870,10 @@
         <v>97.0</v>
       </c>
       <c r="B98" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C98" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D98" t="s">
         <v>114</v>
@@ -3879,7 +3882,7 @@
         <v>105.0</v>
       </c>
       <c r="F98" t="n">
-        <v>3.0</v>
+        <v>8.0</v>
       </c>
       <c r="G98" t="n">
         <v>0.0</v>
@@ -3902,10 +3905,10 @@
         <v>98.0</v>
       </c>
       <c r="B99" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C99" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D99" t="s">
         <v>115</v>
@@ -3937,10 +3940,10 @@
         <v>99.0</v>
       </c>
       <c r="B100" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C100" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D100" t="s">
         <v>116</v>
@@ -3949,10 +3952,10 @@
         <v>105.0</v>
       </c>
       <c r="F100" t="n">
-        <v>39.0</v>
+        <v>3.0</v>
       </c>
       <c r="G100" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="H100" t="n">
         <v>4.0</v>
@@ -3963,8 +3966,8 @@
       <c r="J100" t="b">
         <v>1</v>
       </c>
-      <c r="K100" t="b">
-        <v>1</v>
+      <c r="K100" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="101">
@@ -3972,10 +3975,10 @@
         <v>100.0</v>
       </c>
       <c r="B101" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C101" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D101" t="s">
         <v>117</v>
@@ -3984,10 +3987,10 @@
         <v>105.0</v>
       </c>
       <c r="F101" t="n">
-        <v>8.0</v>
+        <v>39.0</v>
       </c>
       <c r="G101" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="H101" t="n">
         <v>4.0</v>
@@ -3998,8 +4001,8 @@
       <c r="J101" t="b">
         <v>1</v>
       </c>
-      <c r="K101" t="s">
-        <v>14</v>
+      <c r="K101" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="102">
@@ -4007,19 +4010,19 @@
         <v>101.0</v>
       </c>
       <c r="B102" t="s">
+        <v>102</v>
+      </c>
+      <c r="C102" t="s">
+        <v>106</v>
+      </c>
+      <c r="D102" t="s">
         <v>118</v>
       </c>
-      <c r="C102" t="s">
-        <v>119</v>
-      </c>
-      <c r="D102" t="s">
-        <v>120</v>
-      </c>
       <c r="E102" t="n">
-        <v>37.0</v>
+        <v>105.0</v>
       </c>
       <c r="F102" t="n">
-        <v>5.0</v>
+        <v>8.0</v>
       </c>
       <c r="G102" t="n">
         <v>0.0</v>
@@ -4028,7 +4031,7 @@
         <v>4.0</v>
       </c>
       <c r="I102" t="n">
-        <v>2.0</v>
+        <v>12.0</v>
       </c>
       <c r="J102" t="b">
         <v>1</v>
@@ -4042,10 +4045,10 @@
         <v>102.0</v>
       </c>
       <c r="B103" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C103" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D103" t="s">
         <v>121</v>
@@ -4054,10 +4057,10 @@
         <v>37.0</v>
       </c>
       <c r="F103" t="n">
-        <v>19.0</v>
+        <v>5.0</v>
       </c>
       <c r="G103" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="H103" t="n">
         <v>4.0</v>
@@ -4068,8 +4071,8 @@
       <c r="J103" t="b">
         <v>1</v>
       </c>
-      <c r="K103" t="b">
-        <v>1</v>
+      <c r="K103" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="104">
@@ -4077,34 +4080,34 @@
         <v>103.0</v>
       </c>
       <c r="B104" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C104" t="s">
+        <v>120</v>
+      </c>
+      <c r="D104" t="s">
         <v>122</v>
       </c>
-      <c r="D104" t="s">
-        <v>123</v>
-      </c>
       <c r="E104" t="n">
-        <v>96.0</v>
+        <v>37.0</v>
       </c>
       <c r="F104" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="G104" t="n">
         <v>4.0</v>
       </c>
-      <c r="G104" t="n">
-        <v>0.0</v>
-      </c>
       <c r="H104" t="n">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="I104" t="n">
-        <v>12.0</v>
+        <v>2.0</v>
       </c>
       <c r="J104" t="b">
         <v>1</v>
       </c>
-      <c r="K104" t="s">
-        <v>14</v>
+      <c r="K104" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="105">
@@ -4112,10 +4115,10 @@
         <v>104.0</v>
       </c>
       <c r="B105" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C105" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D105" t="s">
         <v>124</v>
@@ -4124,10 +4127,10 @@
         <v>96.0</v>
       </c>
       <c r="F105" t="n">
-        <v>7.0</v>
+        <v>4.0</v>
       </c>
       <c r="G105" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H105" t="n">
         <v>6.0</v>
@@ -4138,8 +4141,8 @@
       <c r="J105" t="b">
         <v>1</v>
       </c>
-      <c r="K105" t="b">
-        <v>1</v>
+      <c r="K105" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="106">
@@ -4147,10 +4150,10 @@
         <v>105.0</v>
       </c>
       <c r="B106" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C106" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D106" t="s">
         <v>125</v>
@@ -4159,10 +4162,10 @@
         <v>96.0</v>
       </c>
       <c r="F106" t="n">
-        <v>4.0</v>
+        <v>7.0</v>
       </c>
       <c r="G106" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H106" t="n">
         <v>6.0</v>
@@ -4173,8 +4176,8 @@
       <c r="J106" t="b">
         <v>1</v>
       </c>
-      <c r="K106" t="s">
-        <v>14</v>
+      <c r="K106" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="107">
@@ -4182,10 +4185,10 @@
         <v>106.0</v>
       </c>
       <c r="B107" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C107" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D107" t="s">
         <v>126</v>
@@ -4217,10 +4220,10 @@
         <v>107.0</v>
       </c>
       <c r="B108" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C108" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D108" t="s">
         <v>127</v>
@@ -4229,10 +4232,10 @@
         <v>96.0</v>
       </c>
       <c r="F108" t="n">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="G108" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H108" t="n">
         <v>6.0</v>
@@ -4243,8 +4246,8 @@
       <c r="J108" t="b">
         <v>1</v>
       </c>
-      <c r="K108" t="b">
-        <v>1</v>
+      <c r="K108" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="109">
@@ -4252,10 +4255,10 @@
         <v>108.0</v>
       </c>
       <c r="B109" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C109" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D109" t="s">
         <v>128</v>
@@ -4264,10 +4267,10 @@
         <v>96.0</v>
       </c>
       <c r="F109" t="n">
-        <v>12.0</v>
+        <v>6.0</v>
       </c>
       <c r="G109" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="H109" t="n">
         <v>6.0</v>
@@ -4287,10 +4290,10 @@
         <v>109.0</v>
       </c>
       <c r="B110" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C110" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D110" t="s">
         <v>129</v>
@@ -4299,10 +4302,10 @@
         <v>96.0</v>
       </c>
       <c r="F110" t="n">
-        <v>9.0</v>
+        <v>12.0</v>
       </c>
       <c r="G110" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="H110" t="n">
         <v>6.0</v>
@@ -4322,22 +4325,22 @@
         <v>110.0</v>
       </c>
       <c r="B111" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C111" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D111" t="s">
-        <v>31</v>
+        <v>130</v>
       </c>
       <c r="E111" t="n">
         <v>96.0</v>
       </c>
       <c r="F111" t="n">
-        <v>26.0</v>
+        <v>9.0</v>
       </c>
       <c r="G111" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H111" t="n">
         <v>6.0</v>
@@ -4348,8 +4351,8 @@
       <c r="J111" t="b">
         <v>1</v>
       </c>
-      <c r="K111" t="s">
-        <v>14</v>
+      <c r="K111" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="112">
@@ -4357,19 +4360,19 @@
         <v>111.0</v>
       </c>
       <c r="B112" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C112" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D112" t="s">
-        <v>130</v>
+        <v>32</v>
       </c>
       <c r="E112" t="n">
         <v>96.0</v>
       </c>
       <c r="F112" t="n">
-        <v>4.0</v>
+        <v>26.0</v>
       </c>
       <c r="G112" t="n">
         <v>0.0</v>
@@ -4392,10 +4395,10 @@
         <v>112.0</v>
       </c>
       <c r="B113" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C113" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D113" t="s">
         <v>131</v>
@@ -4404,7 +4407,7 @@
         <v>96.0</v>
       </c>
       <c r="F113" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="G113" t="n">
         <v>0.0</v>
@@ -4427,10 +4430,10 @@
         <v>113.0</v>
       </c>
       <c r="B114" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C114" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D114" t="s">
         <v>132</v>
@@ -4439,10 +4442,10 @@
         <v>96.0</v>
       </c>
       <c r="F114" t="n">
-        <v>23.0</v>
+        <v>3.0</v>
       </c>
       <c r="G114" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H114" t="n">
         <v>6.0</v>
@@ -4453,8 +4456,8 @@
       <c r="J114" t="b">
         <v>1</v>
       </c>
-      <c r="K114" t="b">
-        <v>1</v>
+      <c r="K114" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="115">
@@ -4462,10 +4465,10 @@
         <v>114.0</v>
       </c>
       <c r="B115" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C115" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D115" t="s">
         <v>133</v>
@@ -4474,10 +4477,10 @@
         <v>96.0</v>
       </c>
       <c r="F115" t="n">
-        <v>17.0</v>
+        <v>23.0</v>
       </c>
       <c r="G115" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H115" t="n">
         <v>6.0</v>
@@ -4488,8 +4491,8 @@
       <c r="J115" t="b">
         <v>1</v>
       </c>
-      <c r="K115" t="s">
-        <v>14</v>
+      <c r="K115" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="116">
@@ -4497,28 +4500,28 @@
         <v>115.0</v>
       </c>
       <c r="B116" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C116" t="s">
+        <v>123</v>
+      </c>
+      <c r="D116" t="s">
         <v>134</v>
       </c>
-      <c r="D116" t="s">
-        <v>130</v>
-      </c>
       <c r="E116" t="n">
-        <v>64.0</v>
+        <v>96.0</v>
       </c>
       <c r="F116" t="n">
-        <v>4.0</v>
+        <v>17.0</v>
       </c>
       <c r="G116" t="n">
         <v>0.0</v>
       </c>
       <c r="H116" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="I116" t="n">
-        <v>4.0</v>
+        <v>12.0</v>
       </c>
       <c r="J116" t="b">
         <v>1</v>
@@ -4532,10 +4535,10 @@
         <v>116.0</v>
       </c>
       <c r="B117" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C117" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D117" t="s">
         <v>131</v>
@@ -4544,7 +4547,7 @@
         <v>64.0</v>
       </c>
       <c r="F117" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="G117" t="n">
         <v>0.0</v>
@@ -4567,10 +4570,10 @@
         <v>117.0</v>
       </c>
       <c r="B118" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C118" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D118" t="s">
         <v>132</v>
@@ -4579,10 +4582,10 @@
         <v>64.0</v>
       </c>
       <c r="F118" t="n">
-        <v>23.0</v>
+        <v>3.0</v>
       </c>
       <c r="G118" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H118" t="n">
         <v>1.0</v>
@@ -4593,8 +4596,8 @@
       <c r="J118" t="b">
         <v>1</v>
       </c>
-      <c r="K118" t="b">
-        <v>1</v>
+      <c r="K118" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="119">
@@ -4602,10 +4605,10 @@
         <v>118.0</v>
       </c>
       <c r="B119" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C119" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D119" t="s">
         <v>133</v>
@@ -4614,10 +4617,10 @@
         <v>64.0</v>
       </c>
       <c r="F119" t="n">
-        <v>17.0</v>
+        <v>23.0</v>
       </c>
       <c r="G119" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H119" t="n">
         <v>1.0</v>
@@ -4628,7 +4631,42 @@
       <c r="J119" t="b">
         <v>1</v>
       </c>
-      <c r="K119" t="s">
+      <c r="K119" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>119.0</v>
+      </c>
+      <c r="B120" t="s">
+        <v>119</v>
+      </c>
+      <c r="C120" t="s">
+        <v>135</v>
+      </c>
+      <c r="D120" t="s">
+        <v>134</v>
+      </c>
+      <c r="E120" t="n">
+        <v>64.0</v>
+      </c>
+      <c r="F120" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="G120" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H120" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I120" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="J120" t="b">
+        <v>1</v>
+      </c>
+      <c r="K120" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Continuação da e avaliação dos code smells
Co-Authored-By: dianamml17 <73841693+dianamml17@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ES-2Sem-2021-Grupo-5_metricas.xlsx
+++ b/ES-2Sem-2021-Grupo-5_metricas.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="133">
   <si>
     <t>MethodID</t>
   </si>
@@ -41,12 +41,6 @@
     <t>NOM_CLASS</t>
   </si>
   <si>
-    <t>Is_God_Class</t>
-  </si>
-  <si>
-    <t>Is_Long_Method</t>
-  </si>
-  <si>
     <t>GUI</t>
   </si>
   <si>
@@ -56,9 +50,6 @@
     <t>ConditionGUI(JComboBox&lt;String&gt; metric, JComboBox&lt;String&gt; thresholdOperator, JTextField thresholdValue)</t>
   </si>
   <si>
-    <t>false</t>
-  </si>
-  <si>
     <t>ConditionGUI(boolean isClassRule)</t>
   </si>
   <si>
@@ -92,7 +83,7 @@
     <t>checkValidRule()</t>
   </si>
   <si>
-    <t>codeSmellsEvaluation(ArrayList&lt;String[]&gt; rulesResults, ArrayList&lt;String&gt; fileResults, int u, int i)</t>
+    <t>codeSmellsEvaluation(ArrayList&lt;String[]&gt; rulesResults, ArrayList&lt;String&gt; fileResults, int u)</t>
   </si>
   <si>
     <t>enableDefaultValue(final JTextField tf, final String defaultValue)</t>
@@ -498,25 +489,19 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
       </c>
       <c r="E2" t="n">
         <v>88.0</v>
@@ -532,12 +517,6 @@
       </c>
       <c r="I2" t="n">
         <v>9.0</v>
-      </c>
-      <c r="J2" t="b">
-        <v>1</v>
-      </c>
-      <c r="K2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3">
@@ -545,13 +524,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
       </c>
       <c r="E3" t="n">
         <v>88.0</v>
@@ -568,25 +547,19 @@
       <c r="I3" t="n">
         <v>9.0</v>
       </c>
-      <c r="J3" t="b">
-        <v>1</v>
-      </c>
-      <c r="K3" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
         <v>3.0</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E4" t="n">
         <v>88.0</v>
@@ -603,25 +576,19 @@
       <c r="I4" t="n">
         <v>9.0</v>
       </c>
-      <c r="J4" t="b">
-        <v>1</v>
-      </c>
-      <c r="K4" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>4.0</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E5" t="n">
         <v>88.0</v>
@@ -637,12 +604,6 @@
       </c>
       <c r="I5" t="n">
         <v>9.0</v>
-      </c>
-      <c r="J5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6">
@@ -650,13 +611,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E6" t="n">
         <v>88.0</v>
@@ -672,12 +633,6 @@
       </c>
       <c r="I6" t="n">
         <v>9.0</v>
-      </c>
-      <c r="J6" t="b">
-        <v>1</v>
-      </c>
-      <c r="K6" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7">
@@ -685,13 +640,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E7" t="n">
         <v>88.0</v>
@@ -707,12 +662,6 @@
       </c>
       <c r="I7" t="n">
         <v>9.0</v>
-      </c>
-      <c r="J7" t="b">
-        <v>1</v>
-      </c>
-      <c r="K7" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8">
@@ -720,13 +669,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E8" t="n">
         <v>88.0</v>
@@ -742,12 +691,6 @@
       </c>
       <c r="I8" t="n">
         <v>9.0</v>
-      </c>
-      <c r="J8" t="b">
-        <v>1</v>
-      </c>
-      <c r="K8" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -755,13 +698,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E9" t="n">
         <v>88.0</v>
@@ -777,12 +720,6 @@
       </c>
       <c r="I9" t="n">
         <v>9.0</v>
-      </c>
-      <c r="J9" t="b">
-        <v>1</v>
-      </c>
-      <c r="K9" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="10">
@@ -790,13 +727,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E10" t="n">
         <v>88.0</v>
@@ -812,12 +749,6 @@
       </c>
       <c r="I10" t="n">
         <v>9.0</v>
-      </c>
-      <c r="J10" t="b">
-        <v>1</v>
-      </c>
-      <c r="K10" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="11">
@@ -825,16 +756,16 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E11" t="n">
-        <v>418.0</v>
+        <v>458.0</v>
       </c>
       <c r="F11" t="n">
         <v>3.0</v>
@@ -843,16 +774,10 @@
         <v>0.0</v>
       </c>
       <c r="H11" t="n">
-        <v>46.0</v>
+        <v>52.0</v>
       </c>
       <c r="I11" t="n">
         <v>11.0</v>
-      </c>
-      <c r="J11" t="b">
-        <v>1</v>
-      </c>
-      <c r="K11" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="12">
@@ -860,16 +785,16 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E12" t="n">
-        <v>418.0</v>
+        <v>458.0</v>
       </c>
       <c r="F12" t="n">
         <v>13.0</v>
@@ -878,16 +803,10 @@
         <v>1.0</v>
       </c>
       <c r="H12" t="n">
-        <v>46.0</v>
+        <v>52.0</v>
       </c>
       <c r="I12" t="n">
         <v>11.0</v>
-      </c>
-      <c r="J12" t="b">
-        <v>1</v>
-      </c>
-      <c r="K12" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -895,34 +814,28 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
         <v>23</v>
       </c>
-      <c r="D13" t="s">
-        <v>26</v>
-      </c>
       <c r="E13" t="n">
-        <v>418.0</v>
+        <v>458.0</v>
       </c>
       <c r="F13" t="n">
-        <v>21.0</v>
+        <v>41.0</v>
       </c>
       <c r="G13" t="n">
-        <v>6.0</v>
+        <v>9.0</v>
       </c>
       <c r="H13" t="n">
-        <v>46.0</v>
+        <v>52.0</v>
       </c>
       <c r="I13" t="n">
         <v>11.0</v>
-      </c>
-      <c r="J13" t="b">
-        <v>1</v>
-      </c>
-      <c r="K13" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -930,16 +843,16 @@
         <v>13.0</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E14" t="n">
-        <v>418.0</v>
+        <v>458.0</v>
       </c>
       <c r="F14" t="n">
         <v>24.0</v>
@@ -948,16 +861,10 @@
         <v>2.0</v>
       </c>
       <c r="H14" t="n">
-        <v>46.0</v>
+        <v>52.0</v>
       </c>
       <c r="I14" t="n">
         <v>11.0</v>
-      </c>
-      <c r="J14" t="b">
-        <v>1</v>
-      </c>
-      <c r="K14" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -965,16 +872,16 @@
         <v>14.0</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E15" t="n">
-        <v>418.0</v>
+        <v>458.0</v>
       </c>
       <c r="F15" t="n">
         <v>5.0</v>
@@ -983,16 +890,10 @@
         <v>1.0</v>
       </c>
       <c r="H15" t="n">
-        <v>46.0</v>
+        <v>52.0</v>
       </c>
       <c r="I15" t="n">
         <v>11.0</v>
-      </c>
-      <c r="J15" t="b">
-        <v>1</v>
-      </c>
-      <c r="K15" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -1000,16 +901,16 @@
         <v>15.0</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E16" t="n">
-        <v>418.0</v>
+        <v>458.0</v>
       </c>
       <c r="F16" t="n">
         <v>8.0</v>
@@ -1018,16 +919,10 @@
         <v>0.0</v>
       </c>
       <c r="H16" t="n">
-        <v>46.0</v>
+        <v>52.0</v>
       </c>
       <c r="I16" t="n">
         <v>11.0</v>
-      </c>
-      <c r="J16" t="b">
-        <v>1</v>
-      </c>
-      <c r="K16" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="17">
@@ -1035,16 +930,16 @@
         <v>16.0</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E17" t="n">
-        <v>418.0</v>
+        <v>458.0</v>
       </c>
       <c r="F17" t="n">
         <v>19.0</v>
@@ -1053,16 +948,10 @@
         <v>4.0</v>
       </c>
       <c r="H17" t="n">
-        <v>46.0</v>
+        <v>52.0</v>
       </c>
       <c r="I17" t="n">
         <v>11.0</v>
-      </c>
-      <c r="J17" t="b">
-        <v>1</v>
-      </c>
-      <c r="K17" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -1070,16 +959,16 @@
         <v>17.0</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D18" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E18" t="n">
-        <v>418.0</v>
+        <v>458.0</v>
       </c>
       <c r="F18" t="n">
         <v>210.0</v>
@@ -1088,16 +977,10 @@
         <v>18.0</v>
       </c>
       <c r="H18" t="n">
-        <v>46.0</v>
+        <v>52.0</v>
       </c>
       <c r="I18" t="n">
         <v>11.0</v>
-      </c>
-      <c r="J18" t="b">
-        <v>1</v>
-      </c>
-      <c r="K18" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -1105,16 +988,16 @@
         <v>18.0</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E19" t="n">
-        <v>418.0</v>
+        <v>458.0</v>
       </c>
       <c r="F19" t="n">
         <v>12.0</v>
@@ -1123,16 +1006,10 @@
         <v>0.0</v>
       </c>
       <c r="H19" t="n">
-        <v>46.0</v>
+        <v>52.0</v>
       </c>
       <c r="I19" t="n">
         <v>11.0</v>
-      </c>
-      <c r="J19" t="b">
-        <v>1</v>
-      </c>
-      <c r="K19" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="20">
@@ -1140,16 +1017,16 @@
         <v>19.0</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D20" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E20" t="n">
-        <v>418.0</v>
+        <v>458.0</v>
       </c>
       <c r="F20" t="n">
         <v>14.0</v>
@@ -1158,16 +1035,10 @@
         <v>1.0</v>
       </c>
       <c r="H20" t="n">
-        <v>46.0</v>
+        <v>52.0</v>
       </c>
       <c r="I20" t="n">
         <v>11.0</v>
-      </c>
-      <c r="J20" t="b">
-        <v>1</v>
-      </c>
-      <c r="K20" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -1175,34 +1046,28 @@
         <v>20.0</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E21" t="n">
-        <v>418.0</v>
+        <v>458.0</v>
       </c>
       <c r="F21" t="n">
-        <v>100.0</v>
+        <v>123.0</v>
       </c>
       <c r="G21" t="n">
-        <v>13.0</v>
+        <v>16.0</v>
       </c>
       <c r="H21" t="n">
-        <v>46.0</v>
+        <v>52.0</v>
       </c>
       <c r="I21" t="n">
         <v>11.0</v>
-      </c>
-      <c r="J21" t="b">
-        <v>1</v>
-      </c>
-      <c r="K21" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -1210,13 +1075,13 @@
         <v>21.0</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D22" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E22" t="n">
         <v>139.0</v>
@@ -1232,12 +1097,6 @@
       </c>
       <c r="I22" t="n">
         <v>11.0</v>
-      </c>
-      <c r="J22" t="b">
-        <v>1</v>
-      </c>
-      <c r="K22" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="23">
@@ -1245,13 +1104,13 @@
         <v>22.0</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D23" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E23" t="n">
         <v>139.0</v>
@@ -1267,12 +1126,6 @@
       </c>
       <c r="I23" t="n">
         <v>11.0</v>
-      </c>
-      <c r="J23" t="b">
-        <v>1</v>
-      </c>
-      <c r="K23" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="24">
@@ -1280,13 +1133,13 @@
         <v>23.0</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" t="s">
         <v>35</v>
-      </c>
-      <c r="D24" t="s">
-        <v>38</v>
       </c>
       <c r="E24" t="n">
         <v>139.0</v>
@@ -1302,12 +1155,6 @@
       </c>
       <c r="I24" t="n">
         <v>11.0</v>
-      </c>
-      <c r="J24" t="b">
-        <v>1</v>
-      </c>
-      <c r="K24" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="25">
@@ -1315,13 +1162,13 @@
         <v>24.0</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D25" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E25" t="n">
         <v>139.0</v>
@@ -1337,12 +1184,6 @@
       </c>
       <c r="I25" t="n">
         <v>11.0</v>
-      </c>
-      <c r="J25" t="b">
-        <v>1</v>
-      </c>
-      <c r="K25" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="26">
@@ -1350,13 +1191,13 @@
         <v>25.0</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D26" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E26" t="n">
         <v>139.0</v>
@@ -1372,12 +1213,6 @@
       </c>
       <c r="I26" t="n">
         <v>11.0</v>
-      </c>
-      <c r="J26" t="b">
-        <v>1</v>
-      </c>
-      <c r="K26" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="27">
@@ -1385,13 +1220,13 @@
         <v>26.0</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D27" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E27" t="n">
         <v>139.0</v>
@@ -1407,12 +1242,6 @@
       </c>
       <c r="I27" t="n">
         <v>11.0</v>
-      </c>
-      <c r="J27" t="b">
-        <v>1</v>
-      </c>
-      <c r="K27" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -1420,13 +1249,13 @@
         <v>27.0</v>
       </c>
       <c r="B28" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D28" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E28" t="n">
         <v>139.0</v>
@@ -1442,12 +1271,6 @@
       </c>
       <c r="I28" t="n">
         <v>11.0</v>
-      </c>
-      <c r="J28" t="b">
-        <v>1</v>
-      </c>
-      <c r="K28" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="29">
@@ -1455,13 +1278,13 @@
         <v>28.0</v>
       </c>
       <c r="B29" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D29" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E29" t="n">
         <v>139.0</v>
@@ -1477,12 +1300,6 @@
       </c>
       <c r="I29" t="n">
         <v>11.0</v>
-      </c>
-      <c r="J29" t="b">
-        <v>1</v>
-      </c>
-      <c r="K29" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="30">
@@ -1490,13 +1307,13 @@
         <v>29.0</v>
       </c>
       <c r="B30" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C30" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D30" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E30" t="n">
         <v>139.0</v>
@@ -1512,12 +1329,6 @@
       </c>
       <c r="I30" t="n">
         <v>11.0</v>
-      </c>
-      <c r="J30" t="b">
-        <v>1</v>
-      </c>
-      <c r="K30" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="31">
@@ -1525,13 +1336,13 @@
         <v>30.0</v>
       </c>
       <c r="B31" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C31" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D31" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E31" t="n">
         <v>139.0</v>
@@ -1547,12 +1358,6 @@
       </c>
       <c r="I31" t="n">
         <v>11.0</v>
-      </c>
-      <c r="J31" t="b">
-        <v>1</v>
-      </c>
-      <c r="K31" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -1560,13 +1365,13 @@
         <v>31.0</v>
       </c>
       <c r="B32" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C32" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D32" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E32" t="n">
         <v>139.0</v>
@@ -1582,12 +1387,6 @@
       </c>
       <c r="I32" t="n">
         <v>11.0</v>
-      </c>
-      <c r="J32" t="b">
-        <v>1</v>
-      </c>
-      <c r="K32" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="33">
@@ -1595,13 +1394,13 @@
         <v>32.0</v>
       </c>
       <c r="B33" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C33" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D33" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E33" t="n">
         <v>69.0</v>
@@ -1617,12 +1416,6 @@
       </c>
       <c r="I33" t="n">
         <v>7.0</v>
-      </c>
-      <c r="J33" t="b">
-        <v>1</v>
-      </c>
-      <c r="K33" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="34">
@@ -1630,13 +1423,13 @@
         <v>33.0</v>
       </c>
       <c r="B34" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C34" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D34" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E34" t="n">
         <v>69.0</v>
@@ -1652,12 +1445,6 @@
       </c>
       <c r="I34" t="n">
         <v>7.0</v>
-      </c>
-      <c r="J34" t="b">
-        <v>1</v>
-      </c>
-      <c r="K34" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="35">
@@ -1665,13 +1452,13 @@
         <v>34.0</v>
       </c>
       <c r="B35" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C35" t="s">
+        <v>43</v>
+      </c>
+      <c r="D35" t="s">
         <v>46</v>
-      </c>
-      <c r="D35" t="s">
-        <v>49</v>
       </c>
       <c r="E35" t="n">
         <v>69.0</v>
@@ -1687,12 +1474,6 @@
       </c>
       <c r="I35" t="n">
         <v>7.0</v>
-      </c>
-      <c r="J35" t="b">
-        <v>1</v>
-      </c>
-      <c r="K35" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="36">
@@ -1700,13 +1481,13 @@
         <v>35.0</v>
       </c>
       <c r="B36" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C36" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D36" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E36" t="n">
         <v>69.0</v>
@@ -1722,12 +1503,6 @@
       </c>
       <c r="I36" t="n">
         <v>7.0</v>
-      </c>
-      <c r="J36" t="b">
-        <v>1</v>
-      </c>
-      <c r="K36" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="37">
@@ -1735,13 +1510,13 @@
         <v>36.0</v>
       </c>
       <c r="B37" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C37" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D37" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E37" t="n">
         <v>69.0</v>
@@ -1757,12 +1532,6 @@
       </c>
       <c r="I37" t="n">
         <v>7.0</v>
-      </c>
-      <c r="J37" t="b">
-        <v>1</v>
-      </c>
-      <c r="K37" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -1770,13 +1539,13 @@
         <v>37.0</v>
       </c>
       <c r="B38" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C38" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D38" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E38" t="n">
         <v>69.0</v>
@@ -1792,12 +1561,6 @@
       </c>
       <c r="I38" t="n">
         <v>7.0</v>
-      </c>
-      <c r="J38" t="b">
-        <v>1</v>
-      </c>
-      <c r="K38" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="39">
@@ -1805,13 +1568,13 @@
         <v>38.0</v>
       </c>
       <c r="B39" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C39" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D39" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E39" t="n">
         <v>69.0</v>
@@ -1827,12 +1590,6 @@
       </c>
       <c r="I39" t="n">
         <v>7.0</v>
-      </c>
-      <c r="J39" t="b">
-        <v>1</v>
-      </c>
-      <c r="K39" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="40">
@@ -1840,13 +1597,13 @@
         <v>39.0</v>
       </c>
       <c r="B40" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C40" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D40" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E40" t="n">
         <v>35.0</v>
@@ -1862,12 +1619,6 @@
       </c>
       <c r="I40" t="n">
         <v>3.0</v>
-      </c>
-      <c r="J40" t="b">
-        <v>1</v>
-      </c>
-      <c r="K40" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="41">
@@ -1875,13 +1626,13 @@
         <v>40.0</v>
       </c>
       <c r="B41" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" t="s">
+        <v>52</v>
+      </c>
+      <c r="D41" t="s">
         <v>54</v>
-      </c>
-      <c r="C41" t="s">
-        <v>55</v>
-      </c>
-      <c r="D41" t="s">
-        <v>57</v>
       </c>
       <c r="E41" t="n">
         <v>35.0</v>
@@ -1897,12 +1648,6 @@
       </c>
       <c r="I41" t="n">
         <v>3.0</v>
-      </c>
-      <c r="J41" t="b">
-        <v>1</v>
-      </c>
-      <c r="K41" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -1910,13 +1655,13 @@
         <v>41.0</v>
       </c>
       <c r="B42" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C42" t="s">
+        <v>52</v>
+      </c>
+      <c r="D42" t="s">
         <v>55</v>
-      </c>
-      <c r="D42" t="s">
-        <v>58</v>
       </c>
       <c r="E42" t="n">
         <v>35.0</v>
@@ -1932,12 +1677,6 @@
       </c>
       <c r="I42" t="n">
         <v>3.0</v>
-      </c>
-      <c r="J42" t="b">
-        <v>1</v>
-      </c>
-      <c r="K42" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="43">
@@ -1945,13 +1684,13 @@
         <v>42.0</v>
       </c>
       <c r="B43" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C43" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D43" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E43" t="n">
         <v>38.0</v>
@@ -1967,12 +1706,6 @@
       </c>
       <c r="I43" t="n">
         <v>4.0</v>
-      </c>
-      <c r="J43" t="b">
-        <v>1</v>
-      </c>
-      <c r="K43" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="44">
@@ -1980,13 +1713,13 @@
         <v>43.0</v>
       </c>
       <c r="B44" t="s">
+        <v>51</v>
+      </c>
+      <c r="C44" t="s">
+        <v>56</v>
+      </c>
+      <c r="D44" t="s">
         <v>54</v>
-      </c>
-      <c r="C44" t="s">
-        <v>59</v>
-      </c>
-      <c r="D44" t="s">
-        <v>57</v>
       </c>
       <c r="E44" t="n">
         <v>38.0</v>
@@ -2002,12 +1735,6 @@
       </c>
       <c r="I44" t="n">
         <v>4.0</v>
-      </c>
-      <c r="J44" t="b">
-        <v>1</v>
-      </c>
-      <c r="K44" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -2015,13 +1742,13 @@
         <v>44.0</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C45" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D45" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E45" t="n">
         <v>38.0</v>
@@ -2037,12 +1764,6 @@
       </c>
       <c r="I45" t="n">
         <v>4.0</v>
-      </c>
-      <c r="J45" t="b">
-        <v>1</v>
-      </c>
-      <c r="K45" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="46">
@@ -2050,13 +1771,13 @@
         <v>45.0</v>
       </c>
       <c r="B46" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C46" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D46" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E46" t="n">
         <v>38.0</v>
@@ -2072,12 +1793,6 @@
       </c>
       <c r="I46" t="n">
         <v>4.0</v>
-      </c>
-      <c r="J46" t="b">
-        <v>1</v>
-      </c>
-      <c r="K46" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="47">
@@ -2085,13 +1800,13 @@
         <v>46.0</v>
       </c>
       <c r="B47" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C47" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D47" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E47" t="n">
         <v>25.0</v>
@@ -2107,12 +1822,6 @@
       </c>
       <c r="I47" t="n">
         <v>3.0</v>
-      </c>
-      <c r="J47" t="b">
-        <v>1</v>
-      </c>
-      <c r="K47" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="48">
@@ -2120,13 +1829,13 @@
         <v>47.0</v>
       </c>
       <c r="B48" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48" t="s">
+        <v>59</v>
+      </c>
+      <c r="D48" t="s">
         <v>54</v>
-      </c>
-      <c r="C48" t="s">
-        <v>62</v>
-      </c>
-      <c r="D48" t="s">
-        <v>57</v>
       </c>
       <c r="E48" t="n">
         <v>25.0</v>
@@ -2142,12 +1851,6 @@
       </c>
       <c r="I48" t="n">
         <v>3.0</v>
-      </c>
-      <c r="J48" t="b">
-        <v>1</v>
-      </c>
-      <c r="K48" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="49">
@@ -2155,13 +1858,13 @@
         <v>48.0</v>
       </c>
       <c r="B49" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C49" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D49" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E49" t="n">
         <v>25.0</v>
@@ -2177,12 +1880,6 @@
       </c>
       <c r="I49" t="n">
         <v>3.0</v>
-      </c>
-      <c r="J49" t="b">
-        <v>1</v>
-      </c>
-      <c r="K49" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="50">
@@ -2190,16 +1887,16 @@
         <v>49.0</v>
       </c>
       <c r="B50" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C50" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D50" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E50" t="n">
-        <v>203.0</v>
+        <v>202.0</v>
       </c>
       <c r="F50" t="n">
         <v>2.0</v>
@@ -2212,12 +1909,6 @@
       </c>
       <c r="I50" t="n">
         <v>20.0</v>
-      </c>
-      <c r="J50" t="b">
-        <v>1</v>
-      </c>
-      <c r="K50" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="51">
@@ -2225,16 +1916,16 @@
         <v>50.0</v>
       </c>
       <c r="B51" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C51" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D51" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E51" t="n">
-        <v>203.0</v>
+        <v>202.0</v>
       </c>
       <c r="F51" t="n">
         <v>5.0</v>
@@ -2247,12 +1938,6 @@
       </c>
       <c r="I51" t="n">
         <v>20.0</v>
-      </c>
-      <c r="J51" t="b">
-        <v>1</v>
-      </c>
-      <c r="K51" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="52">
@@ -2260,16 +1945,16 @@
         <v>51.0</v>
       </c>
       <c r="B52" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C52" t="s">
+        <v>61</v>
+      </c>
+      <c r="D52" t="s">
         <v>64</v>
       </c>
-      <c r="D52" t="s">
-        <v>67</v>
-      </c>
       <c r="E52" t="n">
-        <v>203.0</v>
+        <v>202.0</v>
       </c>
       <c r="F52" t="n">
         <v>3.0</v>
@@ -2282,12 +1967,6 @@
       </c>
       <c r="I52" t="n">
         <v>20.0</v>
-      </c>
-      <c r="J52" t="b">
-        <v>1</v>
-      </c>
-      <c r="K52" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="53">
@@ -2295,16 +1974,16 @@
         <v>52.0</v>
       </c>
       <c r="B53" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C53" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D53" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E53" t="n">
-        <v>203.0</v>
+        <v>202.0</v>
       </c>
       <c r="F53" t="n">
         <v>3.0</v>
@@ -2317,12 +1996,6 @@
       </c>
       <c r="I53" t="n">
         <v>20.0</v>
-      </c>
-      <c r="J53" t="b">
-        <v>1</v>
-      </c>
-      <c r="K53" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="54">
@@ -2330,19 +2003,19 @@
         <v>53.0</v>
       </c>
       <c r="B54" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C54" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D54" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E54" t="n">
-        <v>203.0</v>
+        <v>202.0</v>
       </c>
       <c r="F54" t="n">
-        <v>23.0</v>
+        <v>21.0</v>
       </c>
       <c r="G54" t="n">
         <v>3.0</v>
@@ -2352,12 +2025,6 @@
       </c>
       <c r="I54" t="n">
         <v>20.0</v>
-      </c>
-      <c r="J54" t="b">
-        <v>1</v>
-      </c>
-      <c r="K54" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="55">
@@ -2365,16 +2032,16 @@
         <v>54.0</v>
       </c>
       <c r="B55" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C55" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D55" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E55" t="n">
-        <v>203.0</v>
+        <v>202.0</v>
       </c>
       <c r="F55" t="n">
         <v>13.0</v>
@@ -2387,12 +2054,6 @@
       </c>
       <c r="I55" t="n">
         <v>20.0</v>
-      </c>
-      <c r="J55" t="b">
-        <v>1</v>
-      </c>
-      <c r="K55" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="56">
@@ -2400,19 +2061,19 @@
         <v>55.0</v>
       </c>
       <c r="B56" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C56" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D56" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E56" t="n">
-        <v>203.0</v>
+        <v>202.0</v>
       </c>
       <c r="F56" t="n">
-        <v>41.0</v>
+        <v>42.0</v>
       </c>
       <c r="G56" t="n">
         <v>6.0</v>
@@ -2422,12 +2083,6 @@
       </c>
       <c r="I56" t="n">
         <v>20.0</v>
-      </c>
-      <c r="J56" t="b">
-        <v>1</v>
-      </c>
-      <c r="K56" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="57">
@@ -2435,16 +2090,16 @@
         <v>56.0</v>
       </c>
       <c r="B57" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C57" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D57" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E57" t="n">
-        <v>203.0</v>
+        <v>202.0</v>
       </c>
       <c r="F57" t="n">
         <v>3.0</v>
@@ -2457,12 +2112,6 @@
       </c>
       <c r="I57" t="n">
         <v>20.0</v>
-      </c>
-      <c r="J57" t="b">
-        <v>1</v>
-      </c>
-      <c r="K57" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="58">
@@ -2470,16 +2119,16 @@
         <v>57.0</v>
       </c>
       <c r="B58" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C58" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D58" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E58" t="n">
-        <v>203.0</v>
+        <v>202.0</v>
       </c>
       <c r="F58" t="n">
         <v>3.0</v>
@@ -2492,12 +2141,6 @@
       </c>
       <c r="I58" t="n">
         <v>20.0</v>
-      </c>
-      <c r="J58" t="b">
-        <v>1</v>
-      </c>
-      <c r="K58" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="59">
@@ -2505,16 +2148,16 @@
         <v>58.0</v>
       </c>
       <c r="B59" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C59" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D59" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E59" t="n">
-        <v>203.0</v>
+        <v>202.0</v>
       </c>
       <c r="F59" t="n">
         <v>3.0</v>
@@ -2527,12 +2170,6 @@
       </c>
       <c r="I59" t="n">
         <v>20.0</v>
-      </c>
-      <c r="J59" t="b">
-        <v>1</v>
-      </c>
-      <c r="K59" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="60">
@@ -2540,16 +2177,16 @@
         <v>59.0</v>
       </c>
       <c r="B60" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C60" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D60" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E60" t="n">
-        <v>203.0</v>
+        <v>202.0</v>
       </c>
       <c r="F60" t="n">
         <v>3.0</v>
@@ -2562,12 +2199,6 @@
       </c>
       <c r="I60" t="n">
         <v>20.0</v>
-      </c>
-      <c r="J60" t="b">
-        <v>1</v>
-      </c>
-      <c r="K60" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="61">
@@ -2575,16 +2206,16 @@
         <v>60.0</v>
       </c>
       <c r="B61" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C61" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D61" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E61" t="n">
-        <v>203.0</v>
+        <v>202.0</v>
       </c>
       <c r="F61" t="n">
         <v>3.0</v>
@@ -2597,12 +2228,6 @@
       </c>
       <c r="I61" t="n">
         <v>20.0</v>
-      </c>
-      <c r="J61" t="b">
-        <v>1</v>
-      </c>
-      <c r="K61" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="62">
@@ -2610,16 +2235,16 @@
         <v>61.0</v>
       </c>
       <c r="B62" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C62" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D62" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E62" t="n">
-        <v>203.0</v>
+        <v>202.0</v>
       </c>
       <c r="F62" t="n">
         <v>3.0</v>
@@ -2632,12 +2257,6 @@
       </c>
       <c r="I62" t="n">
         <v>20.0</v>
-      </c>
-      <c r="J62" t="b">
-        <v>1</v>
-      </c>
-      <c r="K62" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="63">
@@ -2645,16 +2264,16 @@
         <v>62.0</v>
       </c>
       <c r="B63" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C63" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D63" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E63" t="n">
-        <v>203.0</v>
+        <v>202.0</v>
       </c>
       <c r="F63" t="n">
         <v>3.0</v>
@@ -2667,12 +2286,6 @@
       </c>
       <c r="I63" t="n">
         <v>20.0</v>
-      </c>
-      <c r="J63" t="b">
-        <v>1</v>
-      </c>
-      <c r="K63" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="64">
@@ -2680,16 +2293,16 @@
         <v>63.0</v>
       </c>
       <c r="B64" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C64" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D64" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E64" t="n">
-        <v>203.0</v>
+        <v>202.0</v>
       </c>
       <c r="F64" t="n">
         <v>3.0</v>
@@ -2702,12 +2315,6 @@
       </c>
       <c r="I64" t="n">
         <v>20.0</v>
-      </c>
-      <c r="J64" t="b">
-        <v>1</v>
-      </c>
-      <c r="K64" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="65">
@@ -2715,16 +2322,16 @@
         <v>64.0</v>
       </c>
       <c r="B65" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C65" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D65" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E65" t="n">
-        <v>203.0</v>
+        <v>202.0</v>
       </c>
       <c r="F65" t="n">
         <v>13.0</v>
@@ -2737,12 +2344,6 @@
       </c>
       <c r="I65" t="n">
         <v>20.0</v>
-      </c>
-      <c r="J65" t="b">
-        <v>1</v>
-      </c>
-      <c r="K65" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="66">
@@ -2750,16 +2351,16 @@
         <v>65.0</v>
       </c>
       <c r="B66" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C66" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D66" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E66" t="n">
-        <v>203.0</v>
+        <v>202.0</v>
       </c>
       <c r="F66" t="n">
         <v>4.0</v>
@@ -2772,12 +2373,6 @@
       </c>
       <c r="I66" t="n">
         <v>20.0</v>
-      </c>
-      <c r="J66" t="b">
-        <v>1</v>
-      </c>
-      <c r="K66" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="67">
@@ -2785,16 +2380,16 @@
         <v>66.0</v>
       </c>
       <c r="B67" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C67" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D67" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E67" t="n">
-        <v>203.0</v>
+        <v>202.0</v>
       </c>
       <c r="F67" t="n">
         <v>42.0</v>
@@ -2807,12 +2402,6 @@
       </c>
       <c r="I67" t="n">
         <v>20.0</v>
-      </c>
-      <c r="J67" t="b">
-        <v>1</v>
-      </c>
-      <c r="K67" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="68">
@@ -2820,16 +2409,16 @@
         <v>67.0</v>
       </c>
       <c r="B68" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C68" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D68" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E68" t="n">
-        <v>203.0</v>
+        <v>202.0</v>
       </c>
       <c r="F68" t="n">
         <v>4.0</v>
@@ -2842,12 +2431,6 @@
       </c>
       <c r="I68" t="n">
         <v>20.0</v>
-      </c>
-      <c r="J68" t="b">
-        <v>1</v>
-      </c>
-      <c r="K68" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="69">
@@ -2855,16 +2438,16 @@
         <v>68.0</v>
       </c>
       <c r="B69" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C69" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D69" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E69" t="n">
-        <v>203.0</v>
+        <v>202.0</v>
       </c>
       <c r="F69" t="n">
         <v>27.0</v>
@@ -2877,12 +2460,6 @@
       </c>
       <c r="I69" t="n">
         <v>20.0</v>
-      </c>
-      <c r="J69" t="b">
-        <v>1</v>
-      </c>
-      <c r="K69" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="70">
@@ -2890,13 +2467,13 @@
         <v>69.0</v>
       </c>
       <c r="B70" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C70" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D70" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E70" t="n">
         <v>167.0</v>
@@ -2912,12 +2489,6 @@
       </c>
       <c r="I70" t="n">
         <v>13.0</v>
-      </c>
-      <c r="J70" t="b">
-        <v>1</v>
-      </c>
-      <c r="K70" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="71">
@@ -2925,13 +2496,13 @@
         <v>70.0</v>
       </c>
       <c r="B71" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C71" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D71" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E71" t="n">
         <v>167.0</v>
@@ -2947,12 +2518,6 @@
       </c>
       <c r="I71" t="n">
         <v>13.0</v>
-      </c>
-      <c r="J71" t="b">
-        <v>1</v>
-      </c>
-      <c r="K71" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="72">
@@ -2960,13 +2525,13 @@
         <v>71.0</v>
       </c>
       <c r="B72" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C72" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D72" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E72" t="n">
         <v>167.0</v>
@@ -2982,12 +2547,6 @@
       </c>
       <c r="I72" t="n">
         <v>13.0</v>
-      </c>
-      <c r="J72" t="b">
-        <v>1</v>
-      </c>
-      <c r="K72" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="73">
@@ -2995,13 +2554,13 @@
         <v>72.0</v>
       </c>
       <c r="B73" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C73" t="s">
+        <v>82</v>
+      </c>
+      <c r="D73" t="s">
         <v>85</v>
-      </c>
-      <c r="D73" t="s">
-        <v>88</v>
       </c>
       <c r="E73" t="n">
         <v>167.0</v>
@@ -3017,12 +2576,6 @@
       </c>
       <c r="I73" t="n">
         <v>13.0</v>
-      </c>
-      <c r="J73" t="b">
-        <v>1</v>
-      </c>
-      <c r="K73" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="74">
@@ -3030,13 +2583,13 @@
         <v>73.0</v>
       </c>
       <c r="B74" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C74" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D74" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E74" t="n">
         <v>167.0</v>
@@ -3052,12 +2605,6 @@
       </c>
       <c r="I74" t="n">
         <v>13.0</v>
-      </c>
-      <c r="J74" t="b">
-        <v>1</v>
-      </c>
-      <c r="K74" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="75">
@@ -3065,13 +2612,13 @@
         <v>74.0</v>
       </c>
       <c r="B75" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C75" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D75" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E75" t="n">
         <v>167.0</v>
@@ -3087,12 +2634,6 @@
       </c>
       <c r="I75" t="n">
         <v>13.0</v>
-      </c>
-      <c r="J75" t="b">
-        <v>1</v>
-      </c>
-      <c r="K75" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="76">
@@ -3100,13 +2641,13 @@
         <v>75.0</v>
       </c>
       <c r="B76" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C76" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D76" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E76" t="n">
         <v>167.0</v>
@@ -3122,12 +2663,6 @@
       </c>
       <c r="I76" t="n">
         <v>13.0</v>
-      </c>
-      <c r="J76" t="b">
-        <v>1</v>
-      </c>
-      <c r="K76" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="77">
@@ -3135,13 +2670,13 @@
         <v>76.0</v>
       </c>
       <c r="B77" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C77" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D77" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E77" t="n">
         <v>167.0</v>
@@ -3157,12 +2692,6 @@
       </c>
       <c r="I77" t="n">
         <v>13.0</v>
-      </c>
-      <c r="J77" t="b">
-        <v>1</v>
-      </c>
-      <c r="K77" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="78">
@@ -3170,13 +2699,13 @@
         <v>77.0</v>
       </c>
       <c r="B78" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C78" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D78" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E78" t="n">
         <v>167.0</v>
@@ -3192,12 +2721,6 @@
       </c>
       <c r="I78" t="n">
         <v>13.0</v>
-      </c>
-      <c r="J78" t="b">
-        <v>1</v>
-      </c>
-      <c r="K78" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="79">
@@ -3205,13 +2728,13 @@
         <v>78.0</v>
       </c>
       <c r="B79" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C79" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D79" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E79" t="n">
         <v>167.0</v>
@@ -3227,12 +2750,6 @@
       </c>
       <c r="I79" t="n">
         <v>13.0</v>
-      </c>
-      <c r="J79" t="b">
-        <v>1</v>
-      </c>
-      <c r="K79" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="80">
@@ -3240,13 +2757,13 @@
         <v>79.0</v>
       </c>
       <c r="B80" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C80" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D80" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E80" t="n">
         <v>167.0</v>
@@ -3262,12 +2779,6 @@
       </c>
       <c r="I80" t="n">
         <v>13.0</v>
-      </c>
-      <c r="J80" t="b">
-        <v>1</v>
-      </c>
-      <c r="K80" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="81">
@@ -3275,13 +2786,13 @@
         <v>80.0</v>
       </c>
       <c r="B81" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C81" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D81" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E81" t="n">
         <v>167.0</v>
@@ -3297,12 +2808,6 @@
       </c>
       <c r="I81" t="n">
         <v>13.0</v>
-      </c>
-      <c r="J81" t="b">
-        <v>1</v>
-      </c>
-      <c r="K81" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="82">
@@ -3310,13 +2815,13 @@
         <v>81.0</v>
       </c>
       <c r="B82" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C82" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D82" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E82" t="n">
         <v>167.0</v>
@@ -3332,12 +2837,6 @@
       </c>
       <c r="I82" t="n">
         <v>13.0</v>
-      </c>
-      <c r="J82" t="b">
-        <v>1</v>
-      </c>
-      <c r="K82" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="83">
@@ -3345,13 +2844,13 @@
         <v>82.0</v>
       </c>
       <c r="B83" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C83" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D83" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E83" t="n">
         <v>25.0</v>
@@ -3367,12 +2866,6 @@
       </c>
       <c r="I83" t="n">
         <v>3.0</v>
-      </c>
-      <c r="J83" t="b">
-        <v>1</v>
-      </c>
-      <c r="K83" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="84">
@@ -3380,13 +2873,13 @@
         <v>83.0</v>
       </c>
       <c r="B84" t="s">
+        <v>51</v>
+      </c>
+      <c r="C84" t="s">
+        <v>95</v>
+      </c>
+      <c r="D84" t="s">
         <v>54</v>
-      </c>
-      <c r="C84" t="s">
-        <v>98</v>
-      </c>
-      <c r="D84" t="s">
-        <v>57</v>
       </c>
       <c r="E84" t="n">
         <v>25.0</v>
@@ -3402,12 +2895,6 @@
       </c>
       <c r="I84" t="n">
         <v>3.0</v>
-      </c>
-      <c r="J84" t="b">
-        <v>1</v>
-      </c>
-      <c r="K84" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="85">
@@ -3415,13 +2902,13 @@
         <v>84.0</v>
       </c>
       <c r="B85" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C85" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D85" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E85" t="n">
         <v>25.0</v>
@@ -3437,12 +2924,6 @@
       </c>
       <c r="I85" t="n">
         <v>3.0</v>
-      </c>
-      <c r="J85" t="b">
-        <v>1</v>
-      </c>
-      <c r="K85" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="86">
@@ -3450,13 +2931,13 @@
         <v>85.0</v>
       </c>
       <c r="B86" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C86" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D86" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E86" t="n">
         <v>25.0</v>
@@ -3472,12 +2953,6 @@
       </c>
       <c r="I86" t="n">
         <v>3.0</v>
-      </c>
-      <c r="J86" t="b">
-        <v>1</v>
-      </c>
-      <c r="K86" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="87">
@@ -3485,13 +2960,13 @@
         <v>86.0</v>
       </c>
       <c r="B87" t="s">
+        <v>51</v>
+      </c>
+      <c r="C87" t="s">
+        <v>97</v>
+      </c>
+      <c r="D87" t="s">
         <v>54</v>
-      </c>
-      <c r="C87" t="s">
-        <v>100</v>
-      </c>
-      <c r="D87" t="s">
-        <v>57</v>
       </c>
       <c r="E87" t="n">
         <v>25.0</v>
@@ -3507,12 +2982,6 @@
       </c>
       <c r="I87" t="n">
         <v>3.0</v>
-      </c>
-      <c r="J87" t="b">
-        <v>1</v>
-      </c>
-      <c r="K87" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="88">
@@ -3520,13 +2989,13 @@
         <v>87.0</v>
       </c>
       <c r="B88" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C88" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D88" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E88" t="n">
         <v>25.0</v>
@@ -3542,12 +3011,6 @@
       </c>
       <c r="I88" t="n">
         <v>3.0</v>
-      </c>
-      <c r="J88" t="b">
-        <v>1</v>
-      </c>
-      <c r="K88" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="89">
@@ -3555,13 +3018,13 @@
         <v>88.0</v>
       </c>
       <c r="B89" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C89" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D89" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E89" t="n">
         <v>42.0</v>
@@ -3577,12 +3040,6 @@
       </c>
       <c r="I89" t="n">
         <v>2.0</v>
-      </c>
-      <c r="J89" t="b">
-        <v>1</v>
-      </c>
-      <c r="K89" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="90">
@@ -3590,13 +3047,13 @@
         <v>89.0</v>
       </c>
       <c r="B90" t="s">
+        <v>99</v>
+      </c>
+      <c r="C90" t="s">
+        <v>100</v>
+      </c>
+      <c r="D90" t="s">
         <v>102</v>
-      </c>
-      <c r="C90" t="s">
-        <v>103</v>
-      </c>
-      <c r="D90" t="s">
-        <v>105</v>
       </c>
       <c r="E90" t="n">
         <v>42.0</v>
@@ -3612,12 +3069,6 @@
       </c>
       <c r="I90" t="n">
         <v>2.0</v>
-      </c>
-      <c r="J90" t="b">
-        <v>1</v>
-      </c>
-      <c r="K90" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="91">
@@ -3625,13 +3076,13 @@
         <v>90.0</v>
       </c>
       <c r="B91" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C91" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D91" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E91" t="n">
         <v>105.0</v>
@@ -3647,12 +3098,6 @@
       </c>
       <c r="I91" t="n">
         <v>12.0</v>
-      </c>
-      <c r="J91" t="b">
-        <v>1</v>
-      </c>
-      <c r="K91" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="92">
@@ -3660,13 +3105,13 @@
         <v>91.0</v>
       </c>
       <c r="B92" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C92" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D92" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E92" t="n">
         <v>105.0</v>
@@ -3682,12 +3127,6 @@
       </c>
       <c r="I92" t="n">
         <v>12.0</v>
-      </c>
-      <c r="J92" t="b">
-        <v>1</v>
-      </c>
-      <c r="K92" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="93">
@@ -3695,13 +3134,13 @@
         <v>92.0</v>
       </c>
       <c r="B93" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C93" t="s">
+        <v>103</v>
+      </c>
+      <c r="D93" t="s">
         <v>106</v>
-      </c>
-      <c r="D93" t="s">
-        <v>109</v>
       </c>
       <c r="E93" t="n">
         <v>105.0</v>
@@ -3717,12 +3156,6 @@
       </c>
       <c r="I93" t="n">
         <v>12.0</v>
-      </c>
-      <c r="J93" t="b">
-        <v>1</v>
-      </c>
-      <c r="K93" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="94">
@@ -3730,13 +3163,13 @@
         <v>93.0</v>
       </c>
       <c r="B94" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C94" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D94" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E94" t="n">
         <v>105.0</v>
@@ -3752,12 +3185,6 @@
       </c>
       <c r="I94" t="n">
         <v>12.0</v>
-      </c>
-      <c r="J94" t="b">
-        <v>1</v>
-      </c>
-      <c r="K94" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="95">
@@ -3765,13 +3192,13 @@
         <v>94.0</v>
       </c>
       <c r="B95" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C95" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D95" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E95" t="n">
         <v>105.0</v>
@@ -3787,12 +3214,6 @@
       </c>
       <c r="I95" t="n">
         <v>12.0</v>
-      </c>
-      <c r="J95" t="b">
-        <v>1</v>
-      </c>
-      <c r="K95" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="96">
@@ -3800,13 +3221,13 @@
         <v>95.0</v>
       </c>
       <c r="B96" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C96" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D96" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E96" t="n">
         <v>105.0</v>
@@ -3822,12 +3243,6 @@
       </c>
       <c r="I96" t="n">
         <v>12.0</v>
-      </c>
-      <c r="J96" t="b">
-        <v>1</v>
-      </c>
-      <c r="K96" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="97">
@@ -3835,13 +3250,13 @@
         <v>96.0</v>
       </c>
       <c r="B97" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C97" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D97" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E97" t="n">
         <v>105.0</v>
@@ -3857,12 +3272,6 @@
       </c>
       <c r="I97" t="n">
         <v>12.0</v>
-      </c>
-      <c r="J97" t="b">
-        <v>1</v>
-      </c>
-      <c r="K97" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="98">
@@ -3870,13 +3279,13 @@
         <v>97.0</v>
       </c>
       <c r="B98" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C98" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D98" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E98" t="n">
         <v>105.0</v>
@@ -3892,12 +3301,6 @@
       </c>
       <c r="I98" t="n">
         <v>12.0</v>
-      </c>
-      <c r="J98" t="b">
-        <v>1</v>
-      </c>
-      <c r="K98" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="99">
@@ -3905,13 +3308,13 @@
         <v>98.0</v>
       </c>
       <c r="B99" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C99" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D99" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E99" t="n">
         <v>105.0</v>
@@ -3927,12 +3330,6 @@
       </c>
       <c r="I99" t="n">
         <v>12.0</v>
-      </c>
-      <c r="J99" t="b">
-        <v>1</v>
-      </c>
-      <c r="K99" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="100">
@@ -3940,13 +3337,13 @@
         <v>99.0</v>
       </c>
       <c r="B100" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C100" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D100" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E100" t="n">
         <v>105.0</v>
@@ -3962,12 +3359,6 @@
       </c>
       <c r="I100" t="n">
         <v>12.0</v>
-      </c>
-      <c r="J100" t="b">
-        <v>1</v>
-      </c>
-      <c r="K100" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="101">
@@ -3975,13 +3366,13 @@
         <v>100.0</v>
       </c>
       <c r="B101" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C101" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D101" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E101" t="n">
         <v>105.0</v>
@@ -3997,12 +3388,6 @@
       </c>
       <c r="I101" t="n">
         <v>12.0</v>
-      </c>
-      <c r="J101" t="b">
-        <v>1</v>
-      </c>
-      <c r="K101" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="102">
@@ -4010,13 +3395,13 @@
         <v>101.0</v>
       </c>
       <c r="B102" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C102" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D102" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E102" t="n">
         <v>105.0</v>
@@ -4032,12 +3417,6 @@
       </c>
       <c r="I102" t="n">
         <v>12.0</v>
-      </c>
-      <c r="J102" t="b">
-        <v>1</v>
-      </c>
-      <c r="K102" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="103">
@@ -4045,13 +3424,13 @@
         <v>102.0</v>
       </c>
       <c r="B103" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C103" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D103" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E103" t="n">
         <v>37.0</v>
@@ -4067,12 +3446,6 @@
       </c>
       <c r="I103" t="n">
         <v>2.0</v>
-      </c>
-      <c r="J103" t="b">
-        <v>1</v>
-      </c>
-      <c r="K103" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="104">
@@ -4080,13 +3453,13 @@
         <v>103.0</v>
       </c>
       <c r="B104" t="s">
+        <v>116</v>
+      </c>
+      <c r="C104" t="s">
+        <v>117</v>
+      </c>
+      <c r="D104" t="s">
         <v>119</v>
-      </c>
-      <c r="C104" t="s">
-        <v>120</v>
-      </c>
-      <c r="D104" t="s">
-        <v>122</v>
       </c>
       <c r="E104" t="n">
         <v>37.0</v>
@@ -4102,12 +3475,6 @@
       </c>
       <c r="I104" t="n">
         <v>2.0</v>
-      </c>
-      <c r="J104" t="b">
-        <v>1</v>
-      </c>
-      <c r="K104" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="105">
@@ -4115,13 +3482,13 @@
         <v>104.0</v>
       </c>
       <c r="B105" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C105" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D105" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E105" t="n">
         <v>96.0</v>
@@ -4137,12 +3504,6 @@
       </c>
       <c r="I105" t="n">
         <v>12.0</v>
-      </c>
-      <c r="J105" t="b">
-        <v>1</v>
-      </c>
-      <c r="K105" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="106">
@@ -4150,13 +3511,13 @@
         <v>105.0</v>
       </c>
       <c r="B106" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C106" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D106" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E106" t="n">
         <v>96.0</v>
@@ -4172,12 +3533,6 @@
       </c>
       <c r="I106" t="n">
         <v>12.0</v>
-      </c>
-      <c r="J106" t="b">
-        <v>1</v>
-      </c>
-      <c r="K106" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="107">
@@ -4185,13 +3540,13 @@
         <v>106.0</v>
       </c>
       <c r="B107" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C107" t="s">
+        <v>120</v>
+      </c>
+      <c r="D107" t="s">
         <v>123</v>
-      </c>
-      <c r="D107" t="s">
-        <v>126</v>
       </c>
       <c r="E107" t="n">
         <v>96.0</v>
@@ -4207,12 +3562,6 @@
       </c>
       <c r="I107" t="n">
         <v>12.0</v>
-      </c>
-      <c r="J107" t="b">
-        <v>1</v>
-      </c>
-      <c r="K107" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="108">
@@ -4220,13 +3569,13 @@
         <v>107.0</v>
       </c>
       <c r="B108" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C108" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D108" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E108" t="n">
         <v>96.0</v>
@@ -4242,12 +3591,6 @@
       </c>
       <c r="I108" t="n">
         <v>12.0</v>
-      </c>
-      <c r="J108" t="b">
-        <v>1</v>
-      </c>
-      <c r="K108" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="109">
@@ -4255,13 +3598,13 @@
         <v>108.0</v>
       </c>
       <c r="B109" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C109" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D109" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E109" t="n">
         <v>96.0</v>
@@ -4277,12 +3620,6 @@
       </c>
       <c r="I109" t="n">
         <v>12.0</v>
-      </c>
-      <c r="J109" t="b">
-        <v>1</v>
-      </c>
-      <c r="K109" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="110">
@@ -4290,13 +3627,13 @@
         <v>109.0</v>
       </c>
       <c r="B110" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C110" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D110" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E110" t="n">
         <v>96.0</v>
@@ -4312,12 +3649,6 @@
       </c>
       <c r="I110" t="n">
         <v>12.0</v>
-      </c>
-      <c r="J110" t="b">
-        <v>1</v>
-      </c>
-      <c r="K110" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="111">
@@ -4325,13 +3656,13 @@
         <v>110.0</v>
       </c>
       <c r="B111" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C111" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D111" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E111" t="n">
         <v>96.0</v>
@@ -4347,12 +3678,6 @@
       </c>
       <c r="I111" t="n">
         <v>12.0</v>
-      </c>
-      <c r="J111" t="b">
-        <v>1</v>
-      </c>
-      <c r="K111" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="112">
@@ -4360,13 +3685,13 @@
         <v>111.0</v>
       </c>
       <c r="B112" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C112" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D112" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E112" t="n">
         <v>96.0</v>
@@ -4382,12 +3707,6 @@
       </c>
       <c r="I112" t="n">
         <v>12.0</v>
-      </c>
-      <c r="J112" t="b">
-        <v>1</v>
-      </c>
-      <c r="K112" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="113">
@@ -4395,13 +3714,13 @@
         <v>112.0</v>
       </c>
       <c r="B113" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C113" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D113" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E113" t="n">
         <v>96.0</v>
@@ -4417,12 +3736,6 @@
       </c>
       <c r="I113" t="n">
         <v>12.0</v>
-      </c>
-      <c r="J113" t="b">
-        <v>1</v>
-      </c>
-      <c r="K113" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="114">
@@ -4430,13 +3743,13 @@
         <v>113.0</v>
       </c>
       <c r="B114" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C114" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D114" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E114" t="n">
         <v>96.0</v>
@@ -4452,12 +3765,6 @@
       </c>
       <c r="I114" t="n">
         <v>12.0</v>
-      </c>
-      <c r="J114" t="b">
-        <v>1</v>
-      </c>
-      <c r="K114" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="115">
@@ -4465,13 +3772,13 @@
         <v>114.0</v>
       </c>
       <c r="B115" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C115" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D115" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E115" t="n">
         <v>96.0</v>
@@ -4487,12 +3794,6 @@
       </c>
       <c r="I115" t="n">
         <v>12.0</v>
-      </c>
-      <c r="J115" t="b">
-        <v>1</v>
-      </c>
-      <c r="K115" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="116">
@@ -4500,13 +3801,13 @@
         <v>115.0</v>
       </c>
       <c r="B116" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C116" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D116" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E116" t="n">
         <v>96.0</v>
@@ -4522,12 +3823,6 @@
       </c>
       <c r="I116" t="n">
         <v>12.0</v>
-      </c>
-      <c r="J116" t="b">
-        <v>1</v>
-      </c>
-      <c r="K116" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="117">
@@ -4535,13 +3830,13 @@
         <v>116.0</v>
       </c>
       <c r="B117" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C117" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D117" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E117" t="n">
         <v>64.0</v>
@@ -4557,12 +3852,6 @@
       </c>
       <c r="I117" t="n">
         <v>4.0</v>
-      </c>
-      <c r="J117" t="b">
-        <v>1</v>
-      </c>
-      <c r="K117" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="118">
@@ -4570,13 +3859,13 @@
         <v>117.0</v>
       </c>
       <c r="B118" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C118" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D118" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E118" t="n">
         <v>64.0</v>
@@ -4592,12 +3881,6 @@
       </c>
       <c r="I118" t="n">
         <v>4.0</v>
-      </c>
-      <c r="J118" t="b">
-        <v>1</v>
-      </c>
-      <c r="K118" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="119">
@@ -4605,13 +3888,13 @@
         <v>118.0</v>
       </c>
       <c r="B119" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C119" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D119" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E119" t="n">
         <v>64.0</v>
@@ -4627,12 +3910,6 @@
       </c>
       <c r="I119" t="n">
         <v>4.0</v>
-      </c>
-      <c r="J119" t="b">
-        <v>1</v>
-      </c>
-      <c r="K119" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="120">
@@ -4640,13 +3917,13 @@
         <v>119.0</v>
       </c>
       <c r="B120" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C120" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D120" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E120" t="n">
         <v>64.0</v>
@@ -4662,12 +3939,6 @@
       </c>
       <c r="I120" t="n">
         <v>4.0</v>
-      </c>
-      <c r="J120" t="b">
-        <v>1</v>
-      </c>
-      <c r="K120" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalização da avaliação da deteção de code smells e adição de novas features à GUI
Co-Authored-By: dcandeias20 <78976610+dcandeias20@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ES-2Sem-2021-Grupo-5_metricas.xlsx
+++ b/ES-2Sem-2021-Grupo-5_metricas.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="135">
   <si>
     <t>MethodID</t>
   </si>
@@ -41,16 +41,19 @@
     <t>NOM_CLASS</t>
   </si>
   <si>
+    <t>sfsfs</t>
+  </si>
+  <si>
     <t>GUI</t>
   </si>
   <si>
     <t>ConditionGUI</t>
   </si>
   <si>
-    <t>ConditionGUI(JComboBox&lt;String&gt; metric, JComboBox&lt;String&gt; thresholdOperator, JTextField thresholdValue)</t>
-  </si>
-  <si>
-    <t>ConditionGUI(boolean isClassRule)</t>
+    <t>ConditionGUI(JComboBox&lt;String&gt;,JComboBox&lt;String&gt;,JTextField)</t>
+  </si>
+  <si>
+    <t>ConditionGUI(boolean)</t>
   </si>
   <si>
     <t>generateCondition()</t>
@@ -65,13 +68,13 @@
     <t>initializePanel()</t>
   </si>
   <si>
-    <t>setDefaultMetric(String defaultMetric)</t>
-  </si>
-  <si>
-    <t>setDefaultThresholdOp(int defaultIndex)</t>
-  </si>
-  <si>
-    <t>setDefaultThresholdValue(String defaultThresholdValue)</t>
+    <t>setDefaultMetric(String)</t>
+  </si>
+  <si>
+    <t>setDefaultThresholdOp(int)</t>
+  </si>
+  <si>
+    <t>setDefaultThresholdValue(String)</t>
   </si>
   <si>
     <t>MainWindow</t>
@@ -83,31 +86,34 @@
     <t>checkValidRule()</t>
   </si>
   <si>
-    <t>codeSmellsEvaluation(ArrayList&lt;String[]&gt; rulesResults, ArrayList&lt;String&gt; fileResults, int u)</t>
-  </si>
-  <si>
-    <t>enableDefaultValue(final JTextField tf, final String defaultValue)</t>
-  </si>
-  <si>
-    <t>getFileName(String fullPath)</t>
-  </si>
-  <si>
-    <t>getPopupImageIcon(String iconPath)</t>
-  </si>
-  <si>
-    <t>getProjectData(ArrayList&lt;Line&gt; lines)</t>
+    <t>codeSmellsEvaluation(ArrayList&lt;String[]&gt;,ArrayList&lt;String&gt;,int,int)</t>
+  </si>
+  <si>
+    <t>comparewithCodeSmellsFile(String[],ArrayList&lt;String[]&gt;)</t>
+  </si>
+  <si>
+    <t>enableDefaultValue(final,tf,,String)</t>
+  </si>
+  <si>
+    <t>getFileName(String)</t>
+  </si>
+  <si>
+    <t>getPopupImageIcon(String)</t>
+  </si>
+  <si>
+    <t>getProjectData(ArrayList&lt;Line&gt;)</t>
   </si>
   <si>
     <t>initialize()</t>
   </si>
   <si>
-    <t>main(String[] args)</t>
-  </si>
-  <si>
-    <t>showFilesToAnalyze(ArrayList&lt;File&gt; fileArray)</t>
-  </si>
-  <si>
-    <t>showImportedData(String fileToImport)</t>
+    <t>main(String[])</t>
+  </si>
+  <si>
+    <t>showFilesToAnalyze(ArrayList&lt;File&gt;)</t>
+  </si>
+  <si>
+    <t>showImportedData(String)</t>
   </si>
   <si>
     <t>RuleGUI</t>
@@ -116,16 +122,16 @@
     <t>JButton()</t>
   </si>
   <si>
-    <t>RuleGUI(JPanel parentPanel, boolean isClassRule)</t>
-  </si>
-  <si>
-    <t>addCondition(ConditionGUI newCondition)</t>
+    <t>RuleGUI(JPanel,boolean)</t>
+  </si>
+  <si>
+    <t>addCondition(ConditionGUI)</t>
   </si>
   <si>
     <t>addNewConditionComboBox()</t>
   </si>
   <si>
-    <t>addNewLogicOperator(int defaultIndex)</t>
+    <t>addNewLogicOperator(int)</t>
   </si>
   <si>
     <t>generateRule()</t>
@@ -149,22 +155,22 @@
     <t>WrapLayout()</t>
   </si>
   <si>
-    <t>WrapLayout(int align)</t>
-  </si>
-  <si>
-    <t>WrapLayout(int align, int hgap, int vgap)</t>
-  </si>
-  <si>
-    <t>addRow(Dimension dim, int rowWidth, int rowHeight)</t>
-  </si>
-  <si>
-    <t>layoutSize(Container target, boolean preferred)</t>
-  </si>
-  <si>
-    <t>minimumLayoutSize(Container target)</t>
-  </si>
-  <si>
-    <t>preferredLayoutSize(Container target)</t>
+    <t>WrapLayout(int)</t>
+  </si>
+  <si>
+    <t>WrapLayout(int,int,int)</t>
+  </si>
+  <si>
+    <t>addRow(Dimension,int,int)</t>
+  </si>
+  <si>
+    <t>layoutSize(Container,boolean)</t>
+  </si>
+  <si>
+    <t>minimumLayoutSize(Container)</t>
+  </si>
+  <si>
+    <t>preferredLayoutSize(Container)</t>
   </si>
   <si>
     <t>metricas</t>
@@ -173,10 +179,10 @@
     <t>CYCLO_method</t>
   </si>
   <si>
-    <t>CYCLO_method(Maestro metricas)</t>
-  </si>
-  <si>
-    <t>applyMetricFilter(String methodCode)</t>
+    <t>CYCLO_method(Maestro)</t>
+  </si>
+  <si>
+    <t>applyMetricFilter(String)</t>
   </si>
   <si>
     <t>extractMetrics()</t>
@@ -185,16 +191,16 @@
     <t>LOC_class</t>
   </si>
   <si>
-    <t>LOC_class(Maestro metricas)</t>
-  </si>
-  <si>
-    <t>filterCode(File file)</t>
+    <t>LOC_class(Maestro)</t>
+  </si>
+  <si>
+    <t>filterCode(File)</t>
   </si>
   <si>
     <t>LOC_method</t>
   </si>
   <si>
-    <t>LOC_method(Maestro metricas)</t>
+    <t>LOC_method(Maestro)</t>
   </si>
   <si>
     <t>Maestro</t>
@@ -203,22 +209,22 @@
     <t>Maestro()</t>
   </si>
   <si>
-    <t>Maestro(String projectDirectory)</t>
-  </si>
-  <si>
-    <t>addRule(Rule rule)</t>
-  </si>
-  <si>
-    <t>addRules(List&lt;Rule&gt; rules)</t>
-  </si>
-  <si>
-    <t>createHeaderExcel(XSSFSheet sheet)</t>
-  </si>
-  <si>
-    <t>cutAbsolutePath(String absolutePath)</t>
-  </si>
-  <si>
-    <t>exportResults(XSSFSheet sheet)</t>
+    <t>Maestro(String)</t>
+  </si>
+  <si>
+    <t>addRule(Rule)</t>
+  </si>
+  <si>
+    <t>addRules(List&lt;Rule&gt;)</t>
+  </si>
+  <si>
+    <t>createHeaderExcel(XSSFSheet)</t>
+  </si>
+  <si>
+    <t>cutAbsolutePath(String)</t>
+  </si>
+  <si>
+    <t>exportResults(XSSFSheet)</t>
   </si>
   <si>
     <t>getCYCLO_method()</t>
@@ -245,10 +251,10 @@
     <t>getWMC_class()</t>
   </si>
   <si>
-    <t>listFilesForFolder(File folder)</t>
-  </si>
-  <si>
-    <t>openFolder(String str)</t>
+    <t>listFilesForFolder(File)</t>
+  </si>
+  <si>
+    <t>openFolder(String)</t>
   </si>
   <si>
     <t>result()</t>
@@ -257,13 +263,13 @@
     <t>startMetricCounters()</t>
   </si>
   <si>
-    <t>writeExcel(XSSFSheet sheet, String[] line)</t>
+    <t>writeExcel(XSSFSheet,String[])</t>
   </si>
   <si>
     <t>Metrica</t>
   </si>
   <si>
-    <t>Metrica(Maestro metricas)</t>
+    <t>Metrica(Maestro)</t>
   </si>
   <si>
     <t>filterOutJunk()</t>
@@ -272,7 +278,7 @@
     <t>getMaestro()</t>
   </si>
   <si>
-    <t>getMethodName(Stack&lt;String&gt; stack)</t>
+    <t>getMethodName(Stack&lt;String&gt;)</t>
   </si>
   <si>
     <t>getMetricName()</t>
@@ -293,7 +299,7 @@
     <t>isClassMetric()</t>
   </si>
   <si>
-    <t>setPackageClassName(String packageClassName)</t>
+    <t>setPackageClassName(String)</t>
   </si>
   <si>
     <t>startExtracting()</t>
@@ -302,13 +308,13 @@
     <t>NOM_class</t>
   </si>
   <si>
-    <t>NOM_class(Maestro metricas)</t>
+    <t>NOM_class(Maestro)</t>
   </si>
   <si>
     <t>WMC_class</t>
   </si>
   <si>
-    <t>WMC_class(Maestro metricas)</t>
+    <t>WMC_class(Maestro)</t>
   </si>
   <si>
     <t>reader</t>
@@ -317,10 +323,10 @@
     <t>ExcelReader</t>
   </si>
   <si>
-    <t>getColumnNames(Iterator&lt;Row&gt; itr)</t>
-  </si>
-  <si>
-    <t>readExcelFile(String fileToImport)</t>
+    <t>getColumnNames(Iterator&lt;Row&gt;)</t>
+  </si>
+  <si>
+    <t>readExcelFile(String)</t>
   </si>
   <si>
     <t>Line</t>
@@ -329,19 +335,19 @@
     <t>Line()</t>
   </si>
   <si>
-    <t>Line(int methodID, String pkg, String cls, String method)</t>
-  </si>
-  <si>
-    <t>Line(int methodID, String pkg, String cls, String method, LinkedHashMap&lt;String, String&gt; metrics)</t>
-  </si>
-  <si>
-    <t>addMetric(String metricName, String metric)</t>
-  </si>
-  <si>
-    <t>addMetrics(HashMap&lt;String, String&gt; metrics)</t>
-  </si>
-  <si>
-    <t>calculateRule(Rule rule)</t>
+    <t>Line(int,String,String,String)</t>
+  </si>
+  <si>
+    <t>Line(int,String,String,String,LinkedHashMap&lt;String,,metrics)</t>
+  </si>
+  <si>
+    <t>addMetric(String,String)</t>
+  </si>
+  <si>
+    <t>addMetrics(HashMap&lt;String,,metrics)</t>
+  </si>
+  <si>
+    <t>calculateRule(Rule)</t>
   </si>
   <si>
     <t>getCls()</t>
@@ -356,7 +362,7 @@
     <t>getPkg()</t>
   </si>
   <si>
-    <t>setValues(Iterator&lt;Cell&gt; columnNameIterator, Iterator&lt;Cell&gt; metricValueIterator)</t>
+    <t>setValues(Iterator&lt;Cell&gt;,Iterator&lt;Cell&gt;)</t>
   </si>
   <si>
     <t>toArray()</t>
@@ -368,37 +374,37 @@
     <t>Condition</t>
   </si>
   <si>
-    <t>Condition(String metricToEvaluate, int thresholdOperator, int thresholdValue)</t>
-  </si>
-  <si>
-    <t>evaluateCondition(Line line)</t>
+    <t>Condition(String,int,int)</t>
+  </si>
+  <si>
+    <t>evaluateCondition(Line)</t>
   </si>
   <si>
     <t>Rule</t>
   </si>
   <si>
-    <t>Rule(String ruleName, Condition condition)</t>
-  </si>
-  <si>
-    <t>Rule(String ruleName, LinkedList&lt;Condition&gt; conditions, LinkedList&lt;Integer&gt; logicOperators)</t>
-  </si>
-  <si>
-    <t>Rule(String ruleName, String metric, int thresholdOperator, int thresholdValue)</t>
-  </si>
-  <si>
-    <t>addCondition(Condition condition, Integer logicOperator)</t>
-  </si>
-  <si>
-    <t>addConditions(List&lt;Condition&gt; conditions, List&lt;Integer&gt; logicOperators)</t>
-  </si>
-  <si>
-    <t>compareConditions(boolean firstConditionValue, int logicOperator, boolean secondConditionValue)</t>
-  </si>
-  <si>
-    <t>evaluateRule(Line lineToEvaluate)</t>
-  </si>
-  <si>
-    <t>RuleHistoryEntry(String timeStamp, List&lt;Rule&gt; rules)</t>
+    <t>Rule(String,Condition)</t>
+  </si>
+  <si>
+    <t>Rule(String,LinkedList&lt;Condition&gt;,LinkedList&lt;Integer&gt;)</t>
+  </si>
+  <si>
+    <t>Rule(String,String,int,int)</t>
+  </si>
+  <si>
+    <t>addCondition(Condition,Integer)</t>
+  </si>
+  <si>
+    <t>addConditions(List&lt;Condition&gt;,List&lt;Integer&gt;)</t>
+  </si>
+  <si>
+    <t>compareConditions(boolean,int,boolean)</t>
+  </si>
+  <si>
+    <t>evaluateRule(Line)</t>
+  </si>
+  <si>
+    <t>RuleHistoryEntry(String,List&lt;Rule&gt;)</t>
   </si>
   <si>
     <t>clearHistory()</t>
@@ -407,7 +413,7 @@
     <t>readRules()</t>
   </si>
   <si>
-    <t>writeEntry(List&lt;Rule&gt; rules)</t>
+    <t>writeEntry(List&lt;Rule&gt;)</t>
   </si>
   <si>
     <t>RuleFileManager</t>
@@ -489,19 +495,22 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" t="n">
         <v>88.0</v>
@@ -517,6 +526,9 @@
       </c>
       <c r="I2" t="n">
         <v>9.0</v>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -524,13 +536,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" t="n">
         <v>88.0</v>
@@ -547,19 +559,22 @@
       <c r="I3" t="n">
         <v>9.0</v>
       </c>
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
         <v>3.0</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E4" t="n">
         <v>88.0</v>
@@ -575,6 +590,9 @@
       </c>
       <c r="I4" t="n">
         <v>9.0</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -582,13 +600,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E5" t="n">
         <v>88.0</v>
@@ -604,6 +622,9 @@
       </c>
       <c r="I5" t="n">
         <v>9.0</v>
+      </c>
+      <c r="J5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -611,13 +632,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E6" t="n">
         <v>88.0</v>
@@ -633,6 +654,9 @@
       </c>
       <c r="I6" t="n">
         <v>9.0</v>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -640,13 +664,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E7" t="n">
         <v>88.0</v>
@@ -662,6 +686,9 @@
       </c>
       <c r="I7" t="n">
         <v>9.0</v>
+      </c>
+      <c r="J7" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -669,13 +696,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E8" t="n">
         <v>88.0</v>
@@ -691,6 +718,9 @@
       </c>
       <c r="I8" t="n">
         <v>9.0</v>
+      </c>
+      <c r="J8" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -698,13 +728,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E9" t="n">
         <v>88.0</v>
@@ -720,6 +750,9 @@
       </c>
       <c r="I9" t="n">
         <v>9.0</v>
+      </c>
+      <c r="J9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -727,13 +760,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E10" t="n">
         <v>88.0</v>
@@ -749,6 +782,9 @@
       </c>
       <c r="I10" t="n">
         <v>9.0</v>
+      </c>
+      <c r="J10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -756,16 +792,16 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E11" t="n">
-        <v>458.0</v>
+        <v>461.0</v>
       </c>
       <c r="F11" t="n">
         <v>3.0</v>
@@ -774,10 +810,13 @@
         <v>0.0</v>
       </c>
       <c r="H11" t="n">
-        <v>52.0</v>
+        <v>51.0</v>
       </c>
       <c r="I11" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
+      </c>
+      <c r="J11" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -785,16 +824,16 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E12" t="n">
-        <v>458.0</v>
+        <v>461.0</v>
       </c>
       <c r="F12" t="n">
         <v>13.0</v>
@@ -803,10 +842,13 @@
         <v>1.0</v>
       </c>
       <c r="H12" t="n">
-        <v>52.0</v>
+        <v>51.0</v>
       </c>
       <c r="I12" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
+      </c>
+      <c r="J12" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -814,28 +856,31 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E13" t="n">
-        <v>458.0</v>
+        <v>461.0</v>
       </c>
       <c r="F13" t="n">
-        <v>41.0</v>
+        <v>43.0</v>
       </c>
       <c r="G13" t="n">
         <v>9.0</v>
       </c>
       <c r="H13" t="n">
-        <v>52.0</v>
+        <v>51.0</v>
       </c>
       <c r="I13" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
+      </c>
+      <c r="J13" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -843,28 +888,31 @@
         <v>13.0</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E14" t="n">
-        <v>458.0</v>
+        <v>461.0</v>
       </c>
       <c r="F14" t="n">
-        <v>24.0</v>
+        <v>81.0</v>
       </c>
       <c r="G14" t="n">
-        <v>2.0</v>
+        <v>13.0</v>
       </c>
       <c r="H14" t="n">
-        <v>52.0</v>
+        <v>51.0</v>
       </c>
       <c r="I14" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
+      </c>
+      <c r="J14" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -872,28 +920,31 @@
         <v>14.0</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E15" t="n">
-        <v>458.0</v>
+        <v>461.0</v>
       </c>
       <c r="F15" t="n">
-        <v>5.0</v>
+        <v>24.0</v>
       </c>
       <c r="G15" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="H15" t="n">
-        <v>52.0</v>
+        <v>51.0</v>
       </c>
       <c r="I15" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
+      </c>
+      <c r="J15" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -901,28 +952,31 @@
         <v>15.0</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E16" t="n">
-        <v>458.0</v>
+        <v>461.0</v>
       </c>
       <c r="F16" t="n">
-        <v>8.0</v>
+        <v>5.0</v>
       </c>
       <c r="G16" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H16" t="n">
-        <v>52.0</v>
+        <v>51.0</v>
       </c>
       <c r="I16" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
+      </c>
+      <c r="J16" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -930,28 +984,31 @@
         <v>16.0</v>
       </c>
       <c r="B17" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E17" t="n">
-        <v>458.0</v>
+        <v>461.0</v>
       </c>
       <c r="F17" t="n">
-        <v>19.0</v>
+        <v>8.0</v>
       </c>
       <c r="G17" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="H17" t="n">
-        <v>52.0</v>
+        <v>51.0</v>
       </c>
       <c r="I17" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
+      </c>
+      <c r="J17" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -959,28 +1016,31 @@
         <v>17.0</v>
       </c>
       <c r="B18" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E18" t="n">
-        <v>458.0</v>
+        <v>461.0</v>
       </c>
       <c r="F18" t="n">
-        <v>210.0</v>
+        <v>19.0</v>
       </c>
       <c r="G18" t="n">
-        <v>18.0</v>
+        <v>4.0</v>
       </c>
       <c r="H18" t="n">
-        <v>52.0</v>
+        <v>51.0</v>
       </c>
       <c r="I18" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
+      </c>
+      <c r="J18" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -988,28 +1048,31 @@
         <v>18.0</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E19" t="n">
-        <v>458.0</v>
+        <v>461.0</v>
       </c>
       <c r="F19" t="n">
+        <v>210.0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="H19" t="n">
+        <v>51.0</v>
+      </c>
+      <c r="I19" t="n">
         <v>12.0</v>
       </c>
-      <c r="G19" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H19" t="n">
-        <v>52.0</v>
-      </c>
-      <c r="I19" t="n">
-        <v>11.0</v>
+      <c r="J19" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -1017,28 +1080,31 @@
         <v>19.0</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E20" t="n">
-        <v>458.0</v>
+        <v>461.0</v>
       </c>
       <c r="F20" t="n">
-        <v>14.0</v>
+        <v>12.0</v>
       </c>
       <c r="G20" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H20" t="n">
-        <v>52.0</v>
+        <v>51.0</v>
       </c>
       <c r="I20" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
+      </c>
+      <c r="J20" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -1046,28 +1112,31 @@
         <v>20.0</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E21" t="n">
-        <v>458.0</v>
+        <v>461.0</v>
       </c>
       <c r="F21" t="n">
-        <v>123.0</v>
+        <v>14.0</v>
       </c>
       <c r="G21" t="n">
-        <v>16.0</v>
+        <v>1.0</v>
       </c>
       <c r="H21" t="n">
-        <v>52.0</v>
+        <v>51.0</v>
       </c>
       <c r="I21" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
+      </c>
+      <c r="J21" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -1075,28 +1144,31 @@
         <v>21.0</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D22" t="s">
         <v>33</v>
       </c>
       <c r="E22" t="n">
-        <v>139.0</v>
+        <v>461.0</v>
       </c>
       <c r="F22" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="G22" t="n">
         <v>2.0</v>
       </c>
-      <c r="G22" t="n">
-        <v>0.0</v>
-      </c>
       <c r="H22" t="n">
-        <v>6.0</v>
+        <v>51.0</v>
       </c>
       <c r="I22" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
+      </c>
+      <c r="J22" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="23">
@@ -1104,28 +1176,31 @@
         <v>22.0</v>
       </c>
       <c r="B23" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E23" t="n">
         <v>139.0</v>
       </c>
       <c r="F23" t="n">
-        <v>42.0</v>
+        <v>2.0</v>
       </c>
       <c r="G23" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H23" t="n">
         <v>6.0</v>
       </c>
       <c r="I23" t="n">
         <v>11.0</v>
+      </c>
+      <c r="J23" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="24">
@@ -1133,28 +1208,31 @@
         <v>23.0</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D24" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E24" t="n">
         <v>139.0</v>
       </c>
       <c r="F24" t="n">
-        <v>3.0</v>
+        <v>42.0</v>
       </c>
       <c r="G24" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H24" t="n">
         <v>6.0</v>
       </c>
       <c r="I24" t="n">
         <v>11.0</v>
+      </c>
+      <c r="J24" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -1162,13 +1240,13 @@
         <v>24.0</v>
       </c>
       <c r="B25" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D25" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E25" t="n">
         <v>139.0</v>
@@ -1184,6 +1262,9 @@
       </c>
       <c r="I25" t="n">
         <v>11.0</v>
+      </c>
+      <c r="J25" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -1191,19 +1272,19 @@
         <v>25.0</v>
       </c>
       <c r="B26" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D26" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E26" t="n">
         <v>139.0</v>
       </c>
       <c r="F26" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="G26" t="n">
         <v>0.0</v>
@@ -1213,6 +1294,9 @@
       </c>
       <c r="I26" t="n">
         <v>11.0</v>
+      </c>
+      <c r="J26" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -1220,28 +1304,31 @@
         <v>26.0</v>
       </c>
       <c r="B27" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D27" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E27" t="n">
         <v>139.0</v>
       </c>
       <c r="F27" t="n">
-        <v>19.0</v>
+        <v>5.0</v>
       </c>
       <c r="G27" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="H27" t="n">
         <v>6.0</v>
       </c>
       <c r="I27" t="n">
         <v>11.0</v>
+      </c>
+      <c r="J27" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -1249,28 +1336,31 @@
         <v>27.0</v>
       </c>
       <c r="B28" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E28" t="n">
         <v>139.0</v>
       </c>
       <c r="F28" t="n">
-        <v>3.0</v>
+        <v>19.0</v>
       </c>
       <c r="G28" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="H28" t="n">
         <v>6.0</v>
       </c>
       <c r="I28" t="n">
         <v>11.0</v>
+      </c>
+      <c r="J28" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="29">
@@ -1278,13 +1368,13 @@
         <v>28.0</v>
       </c>
       <c r="B29" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D29" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E29" t="n">
         <v>139.0</v>
@@ -1300,6 +1390,9 @@
       </c>
       <c r="I29" t="n">
         <v>11.0</v>
+      </c>
+      <c r="J29" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -1307,13 +1400,13 @@
         <v>29.0</v>
       </c>
       <c r="B30" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D30" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E30" t="n">
         <v>139.0</v>
@@ -1329,6 +1422,9 @@
       </c>
       <c r="I30" t="n">
         <v>11.0</v>
+      </c>
+      <c r="J30" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="31">
@@ -1336,28 +1432,31 @@
         <v>30.0</v>
       </c>
       <c r="B31" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D31" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="E31" t="n">
         <v>139.0</v>
       </c>
       <c r="F31" t="n">
-        <v>19.0</v>
+        <v>3.0</v>
       </c>
       <c r="G31" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="H31" t="n">
         <v>6.0</v>
       </c>
       <c r="I31" t="n">
         <v>11.0</v>
+      </c>
+      <c r="J31" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -1365,28 +1464,31 @@
         <v>31.0</v>
       </c>
       <c r="B32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C32" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D32" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="E32" t="n">
         <v>139.0</v>
       </c>
       <c r="F32" t="n">
-        <v>3.0</v>
+        <v>19.0</v>
       </c>
       <c r="G32" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H32" t="n">
         <v>6.0</v>
       </c>
       <c r="I32" t="n">
         <v>11.0</v>
+      </c>
+      <c r="J32" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -1394,16 +1496,16 @@
         <v>32.0</v>
       </c>
       <c r="B33" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C33" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D33" t="s">
         <v>44</v>
       </c>
       <c r="E33" t="n">
-        <v>69.0</v>
+        <v>139.0</v>
       </c>
       <c r="F33" t="n">
         <v>3.0</v>
@@ -1412,10 +1514,13 @@
         <v>0.0</v>
       </c>
       <c r="H33" t="n">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="I33" t="n">
-        <v>7.0</v>
+        <v>11.0</v>
+      </c>
+      <c r="J33" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="34">
@@ -1423,13 +1528,13 @@
         <v>33.0</v>
       </c>
       <c r="B34" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D34" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E34" t="n">
         <v>69.0</v>
@@ -1445,6 +1550,9 @@
       </c>
       <c r="I34" t="n">
         <v>7.0</v>
+      </c>
+      <c r="J34" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="35">
@@ -1452,13 +1560,13 @@
         <v>34.0</v>
       </c>
       <c r="B35" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C35" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D35" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E35" t="n">
         <v>69.0</v>
@@ -1474,6 +1582,9 @@
       </c>
       <c r="I35" t="n">
         <v>7.0</v>
+      </c>
+      <c r="J35" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -1481,28 +1592,31 @@
         <v>35.0</v>
       </c>
       <c r="B36" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C36" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D36" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E36" t="n">
         <v>69.0</v>
       </c>
       <c r="F36" t="n">
-        <v>7.0</v>
+        <v>3.0</v>
       </c>
       <c r="G36" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H36" t="n">
         <v>7.0</v>
       </c>
       <c r="I36" t="n">
         <v>7.0</v>
+      </c>
+      <c r="J36" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="37">
@@ -1510,28 +1624,31 @@
         <v>36.0</v>
       </c>
       <c r="B37" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C37" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D37" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E37" t="n">
         <v>69.0</v>
       </c>
       <c r="F37" t="n">
-        <v>40.0</v>
+        <v>7.0</v>
       </c>
       <c r="G37" t="n">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
       <c r="H37" t="n">
         <v>7.0</v>
       </c>
       <c r="I37" t="n">
         <v>7.0</v>
+      </c>
+      <c r="J37" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -1539,28 +1656,31 @@
         <v>37.0</v>
       </c>
       <c r="B38" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C38" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D38" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E38" t="n">
         <v>69.0</v>
       </c>
       <c r="F38" t="n">
-        <v>5.0</v>
+        <v>40.0</v>
       </c>
       <c r="G38" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
       <c r="H38" t="n">
         <v>7.0</v>
       </c>
       <c r="I38" t="n">
         <v>7.0</v>
+      </c>
+      <c r="J38" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="39">
@@ -1568,19 +1688,19 @@
         <v>38.0</v>
       </c>
       <c r="B39" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C39" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D39" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E39" t="n">
         <v>69.0</v>
       </c>
       <c r="F39" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="G39" t="n">
         <v>0.0</v>
@@ -1590,6 +1710,9 @@
       </c>
       <c r="I39" t="n">
         <v>7.0</v>
+      </c>
+      <c r="J39" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="40">
@@ -1597,28 +1720,31 @@
         <v>39.0</v>
       </c>
       <c r="B40" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="C40" t="s">
+        <v>45</v>
+      </c>
+      <c r="D40" t="s">
         <v>52</v>
       </c>
-      <c r="D40" t="s">
-        <v>53</v>
-      </c>
       <c r="E40" t="n">
-        <v>35.0</v>
+        <v>69.0</v>
       </c>
       <c r="F40" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="G40" t="n">
         <v>0.0</v>
       </c>
       <c r="H40" t="n">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="I40" t="n">
-        <v>3.0</v>
+        <v>7.0</v>
+      </c>
+      <c r="J40" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="41">
@@ -1626,28 +1752,31 @@
         <v>40.0</v>
       </c>
       <c r="B41" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C41" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D41" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E41" t="n">
         <v>35.0</v>
       </c>
       <c r="F41" t="n">
-        <v>17.0</v>
+        <v>5.0</v>
       </c>
       <c r="G41" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="H41" t="n">
         <v>5.0</v>
       </c>
       <c r="I41" t="n">
         <v>3.0</v>
+      </c>
+      <c r="J41" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -1655,28 +1784,31 @@
         <v>41.0</v>
       </c>
       <c r="B42" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C42" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D42" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E42" t="n">
         <v>35.0</v>
       </c>
       <c r="F42" t="n">
-        <v>8.0</v>
+        <v>17.0</v>
       </c>
       <c r="G42" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="H42" t="n">
         <v>5.0</v>
       </c>
       <c r="I42" t="n">
         <v>3.0</v>
+      </c>
+      <c r="J42" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="43">
@@ -1684,28 +1816,31 @@
         <v>42.0</v>
       </c>
       <c r="B43" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C43" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D43" t="s">
         <v>57</v>
       </c>
       <c r="E43" t="n">
-        <v>38.0</v>
+        <v>35.0</v>
       </c>
       <c r="F43" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="G43" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H43" t="n">
         <v>5.0</v>
       </c>
-      <c r="G43" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H43" t="n">
-        <v>4.0</v>
-      </c>
       <c r="I43" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
+      </c>
+      <c r="J43" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="44">
@@ -1713,13 +1848,13 @@
         <v>43.0</v>
       </c>
       <c r="B44" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C44" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D44" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E44" t="n">
         <v>38.0</v>
@@ -1728,13 +1863,16 @@
         <v>5.0</v>
       </c>
       <c r="G44" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H44" t="n">
         <v>4.0</v>
       </c>
       <c r="I44" t="n">
         <v>4.0</v>
+      </c>
+      <c r="J44" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -1742,19 +1880,19 @@
         <v>44.0</v>
       </c>
       <c r="B45" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C45" t="s">
+        <v>58</v>
+      </c>
+      <c r="D45" t="s">
         <v>56</v>
-      </c>
-      <c r="D45" t="s">
-        <v>55</v>
       </c>
       <c r="E45" t="n">
         <v>38.0</v>
       </c>
       <c r="F45" t="n">
-        <v>9.0</v>
+        <v>5.0</v>
       </c>
       <c r="G45" t="n">
         <v>1.0</v>
@@ -1764,6 +1902,9 @@
       </c>
       <c r="I45" t="n">
         <v>4.0</v>
+      </c>
+      <c r="J45" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="46">
@@ -1771,28 +1912,31 @@
         <v>45.0</v>
       </c>
       <c r="B46" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C46" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E46" t="n">
         <v>38.0</v>
       </c>
       <c r="F46" t="n">
-        <v>14.0</v>
+        <v>9.0</v>
       </c>
       <c r="G46" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="H46" t="n">
         <v>4.0</v>
       </c>
       <c r="I46" t="n">
         <v>4.0</v>
+      </c>
+      <c r="J46" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="47">
@@ -1800,28 +1944,31 @@
         <v>46.0</v>
       </c>
       <c r="B47" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D47" t="s">
         <v>60</v>
       </c>
       <c r="E47" t="n">
-        <v>25.0</v>
+        <v>38.0</v>
       </c>
       <c r="F47" t="n">
-        <v>5.0</v>
+        <v>14.0</v>
       </c>
       <c r="G47" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H47" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="I47" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
+      </c>
+      <c r="J47" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="48">
@@ -1829,28 +1976,31 @@
         <v>47.0</v>
       </c>
       <c r="B48" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C48" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D48" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="E48" t="n">
         <v>25.0</v>
       </c>
       <c r="F48" t="n">
-        <v>8.0</v>
+        <v>5.0</v>
       </c>
       <c r="G48" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H48" t="n">
         <v>2.0</v>
       </c>
       <c r="I48" t="n">
         <v>3.0</v>
+      </c>
+      <c r="J48" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="49">
@@ -1858,13 +2008,13 @@
         <v>48.0</v>
       </c>
       <c r="B49" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C49" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D49" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E49" t="n">
         <v>25.0</v>
@@ -1880,6 +2030,9 @@
       </c>
       <c r="I49" t="n">
         <v>3.0</v>
+      </c>
+      <c r="J49" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="50">
@@ -1887,28 +2040,31 @@
         <v>49.0</v>
       </c>
       <c r="B50" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C50" t="s">
         <v>61</v>
       </c>
       <c r="D50" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E50" t="n">
-        <v>202.0</v>
+        <v>25.0</v>
       </c>
       <c r="F50" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="G50" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H50" t="n">
         <v>2.0</v>
       </c>
-      <c r="G50" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H50" t="n">
-        <v>18.0</v>
-      </c>
       <c r="I50" t="n">
-        <v>20.0</v>
+        <v>3.0</v>
+      </c>
+      <c r="J50" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="51">
@@ -1916,19 +2072,19 @@
         <v>50.0</v>
       </c>
       <c r="B51" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C51" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D51" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E51" t="n">
-        <v>202.0</v>
+        <v>201.0</v>
       </c>
       <c r="F51" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c r="G51" t="n">
         <v>0.0</v>
@@ -1938,6 +2094,9 @@
       </c>
       <c r="I51" t="n">
         <v>20.0</v>
+      </c>
+      <c r="J51" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="52">
@@ -1945,19 +2104,19 @@
         <v>51.0</v>
       </c>
       <c r="B52" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C52" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D52" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E52" t="n">
-        <v>202.0</v>
+        <v>201.0</v>
       </c>
       <c r="F52" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="G52" t="n">
         <v>0.0</v>
@@ -1967,6 +2126,9 @@
       </c>
       <c r="I52" t="n">
         <v>20.0</v>
+      </c>
+      <c r="J52" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="53">
@@ -1974,16 +2136,16 @@
         <v>52.0</v>
       </c>
       <c r="B53" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C53" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D53" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E53" t="n">
-        <v>202.0</v>
+        <v>201.0</v>
       </c>
       <c r="F53" t="n">
         <v>3.0</v>
@@ -1996,6 +2158,9 @@
       </c>
       <c r="I53" t="n">
         <v>20.0</v>
+      </c>
+      <c r="J53" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="54">
@@ -2003,28 +2168,31 @@
         <v>53.0</v>
       </c>
       <c r="B54" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C54" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D54" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E54" t="n">
-        <v>202.0</v>
+        <v>201.0</v>
       </c>
       <c r="F54" t="n">
-        <v>21.0</v>
+        <v>3.0</v>
       </c>
       <c r="G54" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="H54" t="n">
         <v>18.0</v>
       </c>
       <c r="I54" t="n">
         <v>20.0</v>
+      </c>
+      <c r="J54" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="55">
@@ -2032,28 +2200,31 @@
         <v>54.0</v>
       </c>
       <c r="B55" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C55" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D55" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E55" t="n">
-        <v>202.0</v>
+        <v>201.0</v>
       </c>
       <c r="F55" t="n">
-        <v>13.0</v>
+        <v>21.0</v>
       </c>
       <c r="G55" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H55" t="n">
         <v>18.0</v>
       </c>
       <c r="I55" t="n">
         <v>20.0</v>
+      </c>
+      <c r="J55" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="56">
@@ -2061,28 +2232,31 @@
         <v>55.0</v>
       </c>
       <c r="B56" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C56" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D56" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E56" t="n">
-        <v>202.0</v>
+        <v>201.0</v>
       </c>
       <c r="F56" t="n">
-        <v>42.0</v>
+        <v>13.0</v>
       </c>
       <c r="G56" t="n">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
       <c r="H56" t="n">
         <v>18.0</v>
       </c>
       <c r="I56" t="n">
         <v>20.0</v>
+      </c>
+      <c r="J56" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="57">
@@ -2090,28 +2264,31 @@
         <v>56.0</v>
       </c>
       <c r="B57" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C57" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D57" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E57" t="n">
-        <v>202.0</v>
+        <v>201.0</v>
       </c>
       <c r="F57" t="n">
-        <v>3.0</v>
+        <v>41.0</v>
       </c>
       <c r="G57" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
       <c r="H57" t="n">
         <v>18.0</v>
       </c>
       <c r="I57" t="n">
         <v>20.0</v>
+      </c>
+      <c r="J57" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="58">
@@ -2119,16 +2296,16 @@
         <v>57.0</v>
       </c>
       <c r="B58" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C58" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D58" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E58" t="n">
-        <v>202.0</v>
+        <v>201.0</v>
       </c>
       <c r="F58" t="n">
         <v>3.0</v>
@@ -2141,6 +2318,9 @@
       </c>
       <c r="I58" t="n">
         <v>20.0</v>
+      </c>
+      <c r="J58" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="59">
@@ -2148,16 +2328,16 @@
         <v>58.0</v>
       </c>
       <c r="B59" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C59" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D59" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E59" t="n">
-        <v>202.0</v>
+        <v>201.0</v>
       </c>
       <c r="F59" t="n">
         <v>3.0</v>
@@ -2170,6 +2350,9 @@
       </c>
       <c r="I59" t="n">
         <v>20.0</v>
+      </c>
+      <c r="J59" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="60">
@@ -2177,16 +2360,16 @@
         <v>59.0</v>
       </c>
       <c r="B60" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C60" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D60" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E60" t="n">
-        <v>202.0</v>
+        <v>201.0</v>
       </c>
       <c r="F60" t="n">
         <v>3.0</v>
@@ -2199,6 +2382,9 @@
       </c>
       <c r="I60" t="n">
         <v>20.0</v>
+      </c>
+      <c r="J60" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="61">
@@ -2206,16 +2392,16 @@
         <v>60.0</v>
       </c>
       <c r="B61" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C61" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D61" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E61" t="n">
-        <v>202.0</v>
+        <v>201.0</v>
       </c>
       <c r="F61" t="n">
         <v>3.0</v>
@@ -2228,6 +2414,9 @@
       </c>
       <c r="I61" t="n">
         <v>20.0</v>
+      </c>
+      <c r="J61" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="62">
@@ -2235,16 +2424,16 @@
         <v>61.0</v>
       </c>
       <c r="B62" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C62" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D62" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E62" t="n">
-        <v>202.0</v>
+        <v>201.0</v>
       </c>
       <c r="F62" t="n">
         <v>3.0</v>
@@ -2257,6 +2446,9 @@
       </c>
       <c r="I62" t="n">
         <v>20.0</v>
+      </c>
+      <c r="J62" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="63">
@@ -2264,16 +2456,16 @@
         <v>62.0</v>
       </c>
       <c r="B63" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C63" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D63" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E63" t="n">
-        <v>202.0</v>
+        <v>201.0</v>
       </c>
       <c r="F63" t="n">
         <v>3.0</v>
@@ -2286,6 +2478,9 @@
       </c>
       <c r="I63" t="n">
         <v>20.0</v>
+      </c>
+      <c r="J63" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="64">
@@ -2293,16 +2488,16 @@
         <v>63.0</v>
       </c>
       <c r="B64" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C64" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D64" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E64" t="n">
-        <v>202.0</v>
+        <v>201.0</v>
       </c>
       <c r="F64" t="n">
         <v>3.0</v>
@@ -2315,6 +2510,9 @@
       </c>
       <c r="I64" t="n">
         <v>20.0</v>
+      </c>
+      <c r="J64" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="65">
@@ -2322,28 +2520,31 @@
         <v>64.0</v>
       </c>
       <c r="B65" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C65" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D65" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E65" t="n">
-        <v>202.0</v>
+        <v>201.0</v>
       </c>
       <c r="F65" t="n">
-        <v>13.0</v>
+        <v>3.0</v>
       </c>
       <c r="G65" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="H65" t="n">
         <v>18.0</v>
       </c>
       <c r="I65" t="n">
         <v>20.0</v>
+      </c>
+      <c r="J65" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="66">
@@ -2351,28 +2552,31 @@
         <v>65.0</v>
       </c>
       <c r="B66" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C66" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D66" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E66" t="n">
-        <v>202.0</v>
+        <v>201.0</v>
       </c>
       <c r="F66" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="G66" t="n">
         <v>4.0</v>
-      </c>
-      <c r="G66" t="n">
-        <v>0.0</v>
       </c>
       <c r="H66" t="n">
         <v>18.0</v>
       </c>
       <c r="I66" t="n">
         <v>20.0</v>
+      </c>
+      <c r="J66" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="67">
@@ -2380,19 +2584,19 @@
         <v>66.0</v>
       </c>
       <c r="B67" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C67" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D67" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E67" t="n">
-        <v>202.0</v>
+        <v>201.0</v>
       </c>
       <c r="F67" t="n">
-        <v>42.0</v>
+        <v>4.0</v>
       </c>
       <c r="G67" t="n">
         <v>0.0</v>
@@ -2402,6 +2606,9 @@
       </c>
       <c r="I67" t="n">
         <v>20.0</v>
+      </c>
+      <c r="J67" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="68">
@@ -2409,19 +2616,19 @@
         <v>67.0</v>
       </c>
       <c r="B68" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C68" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D68" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E68" t="n">
-        <v>202.0</v>
+        <v>201.0</v>
       </c>
       <c r="F68" t="n">
-        <v>4.0</v>
+        <v>42.0</v>
       </c>
       <c r="G68" t="n">
         <v>0.0</v>
@@ -2431,6 +2638,9 @@
       </c>
       <c r="I68" t="n">
         <v>20.0</v>
+      </c>
+      <c r="J68" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="69">
@@ -2438,28 +2648,31 @@
         <v>68.0</v>
       </c>
       <c r="B69" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C69" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D69" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E69" t="n">
-        <v>202.0</v>
+        <v>201.0</v>
       </c>
       <c r="F69" t="n">
-        <v>27.0</v>
+        <v>4.0</v>
       </c>
       <c r="G69" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="H69" t="n">
         <v>18.0</v>
       </c>
       <c r="I69" t="n">
         <v>20.0</v>
+      </c>
+      <c r="J69" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="70">
@@ -2467,28 +2680,31 @@
         <v>69.0</v>
       </c>
       <c r="B70" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C70" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D70" t="s">
         <v>83</v>
       </c>
       <c r="E70" t="n">
-        <v>167.0</v>
+        <v>201.0</v>
       </c>
       <c r="F70" t="n">
-        <v>6.0</v>
+        <v>27.0</v>
       </c>
       <c r="G70" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="H70" t="n">
-        <v>23.0</v>
+        <v>18.0</v>
       </c>
       <c r="I70" t="n">
-        <v>13.0</v>
+        <v>20.0</v>
+      </c>
+      <c r="J70" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="71">
@@ -2496,28 +2712,31 @@
         <v>70.0</v>
       </c>
       <c r="B71" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C71" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D71" t="s">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="E71" t="n">
-        <v>167.0</v>
+        <v>176.0</v>
       </c>
       <c r="F71" t="n">
-        <v>37.0</v>
+        <v>6.0</v>
       </c>
       <c r="G71" t="n">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
       <c r="H71" t="n">
-        <v>23.0</v>
+        <v>25.0</v>
       </c>
       <c r="I71" t="n">
         <v>13.0</v>
+      </c>
+      <c r="J71" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="72">
@@ -2525,28 +2744,31 @@
         <v>71.0</v>
       </c>
       <c r="B72" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C72" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D72" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="E72" t="n">
-        <v>167.0</v>
+        <v>176.0</v>
       </c>
       <c r="F72" t="n">
-        <v>21.0</v>
+        <v>37.0</v>
       </c>
       <c r="G72" t="n">
-        <v>5.0</v>
+        <v>8.0</v>
       </c>
       <c r="H72" t="n">
-        <v>23.0</v>
+        <v>25.0</v>
       </c>
       <c r="I72" t="n">
         <v>13.0</v>
+      </c>
+      <c r="J72" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="73">
@@ -2554,28 +2776,31 @@
         <v>72.0</v>
       </c>
       <c r="B73" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C73" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D73" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E73" t="n">
-        <v>167.0</v>
+        <v>176.0</v>
       </c>
       <c r="F73" t="n">
-        <v>3.0</v>
+        <v>21.0</v>
       </c>
       <c r="G73" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="H73" t="n">
-        <v>23.0</v>
+        <v>25.0</v>
       </c>
       <c r="I73" t="n">
         <v>13.0</v>
+      </c>
+      <c r="J73" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="74">
@@ -2583,28 +2808,31 @@
         <v>73.0</v>
       </c>
       <c r="B74" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C74" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D74" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E74" t="n">
-        <v>167.0</v>
+        <v>176.0</v>
       </c>
       <c r="F74" t="n">
-        <v>16.0</v>
+        <v>3.0</v>
       </c>
       <c r="G74" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="H74" t="n">
-        <v>23.0</v>
+        <v>25.0</v>
       </c>
       <c r="I74" t="n">
         <v>13.0</v>
+      </c>
+      <c r="J74" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="75">
@@ -2612,28 +2840,31 @@
         <v>74.0</v>
       </c>
       <c r="B75" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C75" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D75" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E75" t="n">
-        <v>167.0</v>
+        <v>176.0</v>
       </c>
       <c r="F75" t="n">
-        <v>3.0</v>
+        <v>25.0</v>
       </c>
       <c r="G75" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="H75" t="n">
-        <v>23.0</v>
+        <v>25.0</v>
       </c>
       <c r="I75" t="n">
         <v>13.0</v>
+      </c>
+      <c r="J75" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="76">
@@ -2641,16 +2872,16 @@
         <v>75.0</v>
       </c>
       <c r="B76" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C76" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D76" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E76" t="n">
-        <v>167.0</v>
+        <v>176.0</v>
       </c>
       <c r="F76" t="n">
         <v>3.0</v>
@@ -2659,10 +2890,13 @@
         <v>0.0</v>
       </c>
       <c r="H76" t="n">
-        <v>23.0</v>
+        <v>25.0</v>
       </c>
       <c r="I76" t="n">
         <v>13.0</v>
+      </c>
+      <c r="J76" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="77">
@@ -2670,16 +2904,16 @@
         <v>76.0</v>
       </c>
       <c r="B77" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C77" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D77" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E77" t="n">
-        <v>167.0</v>
+        <v>176.0</v>
       </c>
       <c r="F77" t="n">
         <v>3.0</v>
@@ -2688,10 +2922,13 @@
         <v>0.0</v>
       </c>
       <c r="H77" t="n">
-        <v>23.0</v>
+        <v>25.0</v>
       </c>
       <c r="I77" t="n">
         <v>13.0</v>
+      </c>
+      <c r="J77" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="78">
@@ -2699,28 +2936,31 @@
         <v>77.0</v>
       </c>
       <c r="B78" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C78" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D78" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E78" t="n">
-        <v>167.0</v>
+        <v>176.0</v>
       </c>
       <c r="F78" t="n">
-        <v>23.0</v>
+        <v>3.0</v>
       </c>
       <c r="G78" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="H78" t="n">
-        <v>23.0</v>
+        <v>25.0</v>
       </c>
       <c r="I78" t="n">
         <v>13.0</v>
+      </c>
+      <c r="J78" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="79">
@@ -2728,28 +2968,31 @@
         <v>78.0</v>
       </c>
       <c r="B79" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C79" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D79" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E79" t="n">
-        <v>167.0</v>
+        <v>176.0</v>
       </c>
       <c r="F79" t="n">
-        <v>24.0</v>
+        <v>23.0</v>
       </c>
       <c r="G79" t="n">
         <v>4.0</v>
       </c>
       <c r="H79" t="n">
-        <v>23.0</v>
+        <v>25.0</v>
       </c>
       <c r="I79" t="n">
         <v>13.0</v>
+      </c>
+      <c r="J79" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="80">
@@ -2757,28 +3000,31 @@
         <v>79.0</v>
       </c>
       <c r="B80" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C80" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D80" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E80" t="n">
-        <v>167.0</v>
+        <v>176.0</v>
       </c>
       <c r="F80" t="n">
-        <v>3.0</v>
+        <v>24.0</v>
       </c>
       <c r="G80" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="H80" t="n">
-        <v>23.0</v>
+        <v>25.0</v>
       </c>
       <c r="I80" t="n">
         <v>13.0</v>
+      </c>
+      <c r="J80" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="81">
@@ -2786,16 +3032,16 @@
         <v>80.0</v>
       </c>
       <c r="B81" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C81" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D81" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E81" t="n">
-        <v>167.0</v>
+        <v>176.0</v>
       </c>
       <c r="F81" t="n">
         <v>3.0</v>
@@ -2804,10 +3050,13 @@
         <v>0.0</v>
       </c>
       <c r="H81" t="n">
-        <v>23.0</v>
+        <v>25.0</v>
       </c>
       <c r="I81" t="n">
         <v>13.0</v>
+      </c>
+      <c r="J81" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="82">
@@ -2815,28 +3064,31 @@
         <v>81.0</v>
       </c>
       <c r="B82" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C82" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D82" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E82" t="n">
-        <v>167.0</v>
+        <v>176.0</v>
       </c>
       <c r="F82" t="n">
-        <v>8.0</v>
+        <v>3.0</v>
       </c>
       <c r="G82" t="n">
         <v>0.0</v>
       </c>
       <c r="H82" t="n">
-        <v>23.0</v>
+        <v>25.0</v>
       </c>
       <c r="I82" t="n">
         <v>13.0</v>
+      </c>
+      <c r="J82" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="83">
@@ -2844,28 +3096,31 @@
         <v>82.0</v>
       </c>
       <c r="B83" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C83" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="D83" t="s">
         <v>96</v>
       </c>
       <c r="E83" t="n">
+        <v>176.0</v>
+      </c>
+      <c r="F83" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="G83" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H83" t="n">
         <v>25.0</v>
       </c>
-      <c r="F83" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="G83" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H83" t="n">
-        <v>3.0</v>
-      </c>
       <c r="I83" t="n">
-        <v>3.0</v>
+        <v>13.0</v>
+      </c>
+      <c r="J83" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="84">
@@ -2873,19 +3128,19 @@
         <v>83.0</v>
       </c>
       <c r="B84" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C84" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D84" t="s">
-        <v>54</v>
+        <v>98</v>
       </c>
       <c r="E84" t="n">
         <v>25.0</v>
       </c>
       <c r="F84" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="G84" t="n">
         <v>0.0</v>
@@ -2895,6 +3150,9 @@
       </c>
       <c r="I84" t="n">
         <v>3.0</v>
+      </c>
+      <c r="J84" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="85">
@@ -2902,28 +3160,31 @@
         <v>84.0</v>
       </c>
       <c r="B85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C85" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D85" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E85" t="n">
         <v>25.0</v>
       </c>
       <c r="F85" t="n">
-        <v>14.0</v>
+        <v>2.0</v>
       </c>
       <c r="G85" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="H85" t="n">
         <v>3.0</v>
       </c>
       <c r="I85" t="n">
         <v>3.0</v>
+      </c>
+      <c r="J85" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="86">
@@ -2931,28 +3192,31 @@
         <v>85.0</v>
       </c>
       <c r="B86" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C86" t="s">
         <v>97</v>
       </c>
       <c r="D86" t="s">
-        <v>98</v>
+        <v>57</v>
       </c>
       <c r="E86" t="n">
         <v>25.0</v>
       </c>
       <c r="F86" t="n">
-        <v>5.0</v>
+        <v>14.0</v>
       </c>
       <c r="G86" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="H86" t="n">
         <v>3.0</v>
       </c>
       <c r="I86" t="n">
         <v>3.0</v>
+      </c>
+      <c r="J86" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="87">
@@ -2960,19 +3224,19 @@
         <v>86.0</v>
       </c>
       <c r="B87" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C87" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D87" t="s">
-        <v>54</v>
+        <v>100</v>
       </c>
       <c r="E87" t="n">
         <v>25.0</v>
       </c>
       <c r="F87" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="G87" t="n">
         <v>0.0</v>
@@ -2982,6 +3246,9 @@
       </c>
       <c r="I87" t="n">
         <v>3.0</v>
+      </c>
+      <c r="J87" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="88">
@@ -2989,28 +3256,31 @@
         <v>87.0</v>
       </c>
       <c r="B88" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C88" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D88" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E88" t="n">
         <v>25.0</v>
       </c>
       <c r="F88" t="n">
-        <v>16.0</v>
+        <v>2.0</v>
       </c>
       <c r="G88" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="H88" t="n">
         <v>3.0</v>
       </c>
       <c r="I88" t="n">
         <v>3.0</v>
+      </c>
+      <c r="J88" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="89">
@@ -3018,28 +3288,31 @@
         <v>88.0</v>
       </c>
       <c r="B89" t="s">
+        <v>53</v>
+      </c>
+      <c r="C89" t="s">
         <v>99</v>
       </c>
-      <c r="C89" t="s">
-        <v>100</v>
-      </c>
       <c r="D89" t="s">
-        <v>101</v>
+        <v>57</v>
       </c>
       <c r="E89" t="n">
-        <v>42.0</v>
+        <v>25.0</v>
       </c>
       <c r="F89" t="n">
-        <v>9.0</v>
+        <v>16.0</v>
       </c>
       <c r="G89" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H89" t="n">
         <v>3.0</v>
       </c>
       <c r="I89" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
+      </c>
+      <c r="J89" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="90">
@@ -3047,28 +3320,31 @@
         <v>89.0</v>
       </c>
       <c r="B90" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C90" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D90" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E90" t="n">
         <v>42.0</v>
       </c>
       <c r="F90" t="n">
-        <v>29.0</v>
+        <v>9.0</v>
       </c>
       <c r="G90" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="H90" t="n">
         <v>3.0</v>
       </c>
       <c r="I90" t="n">
         <v>2.0</v>
+      </c>
+      <c r="J90" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="91">
@@ -3076,28 +3352,31 @@
         <v>90.0</v>
       </c>
       <c r="B91" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C91" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D91" t="s">
         <v>104</v>
       </c>
       <c r="E91" t="n">
-        <v>105.0</v>
+        <v>42.0</v>
       </c>
       <c r="F91" t="n">
-        <v>3.0</v>
+        <v>29.0</v>
       </c>
       <c r="G91" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H91" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="I91" t="n">
-        <v>12.0</v>
+        <v>2.0</v>
+      </c>
+      <c r="J91" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="92">
@@ -3105,19 +3384,19 @@
         <v>91.0</v>
       </c>
       <c r="B92" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C92" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D92" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E92" t="n">
         <v>105.0</v>
       </c>
       <c r="F92" t="n">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="G92" t="n">
         <v>0.0</v>
@@ -3127,6 +3406,9 @@
       </c>
       <c r="I92" t="n">
         <v>12.0</v>
+      </c>
+      <c r="J92" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="93">
@@ -3134,19 +3416,19 @@
         <v>92.0</v>
       </c>
       <c r="B93" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C93" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D93" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E93" t="n">
         <v>105.0</v>
       </c>
       <c r="F93" t="n">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="G93" t="n">
         <v>0.0</v>
@@ -3156,6 +3438,9 @@
       </c>
       <c r="I93" t="n">
         <v>12.0</v>
+      </c>
+      <c r="J93" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="94">
@@ -3163,19 +3448,19 @@
         <v>93.0</v>
       </c>
       <c r="B94" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C94" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D94" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E94" t="n">
         <v>105.0</v>
       </c>
       <c r="F94" t="n">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="G94" t="n">
         <v>0.0</v>
@@ -3185,6 +3470,9 @@
       </c>
       <c r="I94" t="n">
         <v>12.0</v>
+      </c>
+      <c r="J94" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="95">
@@ -3192,13 +3480,13 @@
         <v>94.0</v>
       </c>
       <c r="B95" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C95" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D95" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E95" t="n">
         <v>105.0</v>
@@ -3214,6 +3502,9 @@
       </c>
       <c r="I95" t="n">
         <v>12.0</v>
+      </c>
+      <c r="J95" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="96">
@@ -3221,13 +3512,13 @@
         <v>95.0</v>
       </c>
       <c r="B96" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C96" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D96" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E96" t="n">
         <v>105.0</v>
@@ -3243,6 +3534,9 @@
       </c>
       <c r="I96" t="n">
         <v>12.0</v>
+      </c>
+      <c r="J96" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="97">
@@ -3250,13 +3544,13 @@
         <v>96.0</v>
       </c>
       <c r="B97" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C97" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D97" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E97" t="n">
         <v>105.0</v>
@@ -3272,6 +3566,9 @@
       </c>
       <c r="I97" t="n">
         <v>12.0</v>
+      </c>
+      <c r="J97" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="98">
@@ -3279,19 +3576,19 @@
         <v>97.0</v>
       </c>
       <c r="B98" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C98" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D98" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E98" t="n">
         <v>105.0</v>
       </c>
       <c r="F98" t="n">
-        <v>8.0</v>
+        <v>3.0</v>
       </c>
       <c r="G98" t="n">
         <v>0.0</v>
@@ -3301,6 +3598,9 @@
       </c>
       <c r="I98" t="n">
         <v>12.0</v>
+      </c>
+      <c r="J98" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="99">
@@ -3308,19 +3608,19 @@
         <v>98.0</v>
       </c>
       <c r="B99" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C99" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D99" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E99" t="n">
         <v>105.0</v>
       </c>
       <c r="F99" t="n">
-        <v>3.0</v>
+        <v>8.0</v>
       </c>
       <c r="G99" t="n">
         <v>0.0</v>
@@ -3330,6 +3630,9 @@
       </c>
       <c r="I99" t="n">
         <v>12.0</v>
+      </c>
+      <c r="J99" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="100">
@@ -3337,13 +3640,13 @@
         <v>99.0</v>
       </c>
       <c r="B100" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C100" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D100" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E100" t="n">
         <v>105.0</v>
@@ -3359,6 +3662,9 @@
       </c>
       <c r="I100" t="n">
         <v>12.0</v>
+      </c>
+      <c r="J100" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="101">
@@ -3366,28 +3672,31 @@
         <v>100.0</v>
       </c>
       <c r="B101" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C101" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D101" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E101" t="n">
         <v>105.0</v>
       </c>
       <c r="F101" t="n">
-        <v>39.0</v>
+        <v>3.0</v>
       </c>
       <c r="G101" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="H101" t="n">
         <v>4.0</v>
       </c>
       <c r="I101" t="n">
         <v>12.0</v>
+      </c>
+      <c r="J101" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="102">
@@ -3395,28 +3704,31 @@
         <v>101.0</v>
       </c>
       <c r="B102" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C102" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D102" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E102" t="n">
         <v>105.0</v>
       </c>
       <c r="F102" t="n">
-        <v>8.0</v>
+        <v>39.0</v>
       </c>
       <c r="G102" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="H102" t="n">
         <v>4.0</v>
       </c>
       <c r="I102" t="n">
         <v>12.0</v>
+      </c>
+      <c r="J102" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="103">
@@ -3424,19 +3736,19 @@
         <v>102.0</v>
       </c>
       <c r="B103" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="C103" t="s">
+        <v>105</v>
+      </c>
+      <c r="D103" t="s">
         <v>117</v>
       </c>
-      <c r="D103" t="s">
-        <v>118</v>
-      </c>
       <c r="E103" t="n">
-        <v>37.0</v>
+        <v>105.0</v>
       </c>
       <c r="F103" t="n">
-        <v>5.0</v>
+        <v>8.0</v>
       </c>
       <c r="G103" t="n">
         <v>0.0</v>
@@ -3445,7 +3757,10 @@
         <v>4.0</v>
       </c>
       <c r="I103" t="n">
-        <v>2.0</v>
+        <v>12.0</v>
+      </c>
+      <c r="J103" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="104">
@@ -3453,28 +3768,31 @@
         <v>103.0</v>
       </c>
       <c r="B104" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C104" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D104" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E104" t="n">
         <v>37.0</v>
       </c>
       <c r="F104" t="n">
-        <v>19.0</v>
+        <v>5.0</v>
       </c>
       <c r="G104" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="H104" t="n">
         <v>4.0</v>
       </c>
       <c r="I104" t="n">
         <v>2.0</v>
+      </c>
+      <c r="J104" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="105">
@@ -3482,28 +3800,31 @@
         <v>104.0</v>
       </c>
       <c r="B105" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C105" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D105" t="s">
         <v>121</v>
       </c>
       <c r="E105" t="n">
-        <v>96.0</v>
+        <v>37.0</v>
       </c>
       <c r="F105" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="G105" t="n">
         <v>4.0</v>
       </c>
-      <c r="G105" t="n">
-        <v>0.0</v>
-      </c>
       <c r="H105" t="n">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="I105" t="n">
-        <v>12.0</v>
+        <v>2.0</v>
+      </c>
+      <c r="J105" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="106">
@@ -3511,28 +3832,31 @@
         <v>105.0</v>
       </c>
       <c r="B106" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C106" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D106" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E106" t="n">
         <v>96.0</v>
       </c>
       <c r="F106" t="n">
-        <v>7.0</v>
+        <v>4.0</v>
       </c>
       <c r="G106" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H106" t="n">
         <v>6.0</v>
       </c>
       <c r="I106" t="n">
         <v>12.0</v>
+      </c>
+      <c r="J106" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="107">
@@ -3540,28 +3864,31 @@
         <v>106.0</v>
       </c>
       <c r="B107" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C107" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D107" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E107" t="n">
         <v>96.0</v>
       </c>
       <c r="F107" t="n">
-        <v>4.0</v>
+        <v>7.0</v>
       </c>
       <c r="G107" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H107" t="n">
         <v>6.0</v>
       </c>
       <c r="I107" t="n">
         <v>12.0</v>
+      </c>
+      <c r="J107" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="108">
@@ -3569,13 +3896,13 @@
         <v>107.0</v>
       </c>
       <c r="B108" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C108" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D108" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E108" t="n">
         <v>96.0</v>
@@ -3591,6 +3918,9 @@
       </c>
       <c r="I108" t="n">
         <v>12.0</v>
+      </c>
+      <c r="J108" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="109">
@@ -3598,28 +3928,31 @@
         <v>108.0</v>
       </c>
       <c r="B109" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C109" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D109" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E109" t="n">
         <v>96.0</v>
       </c>
       <c r="F109" t="n">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="G109" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H109" t="n">
         <v>6.0</v>
       </c>
       <c r="I109" t="n">
         <v>12.0</v>
+      </c>
+      <c r="J109" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="110">
@@ -3627,28 +3960,31 @@
         <v>109.0</v>
       </c>
       <c r="B110" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C110" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D110" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E110" t="n">
         <v>96.0</v>
       </c>
       <c r="F110" t="n">
-        <v>12.0</v>
+        <v>6.0</v>
       </c>
       <c r="G110" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="H110" t="n">
         <v>6.0</v>
       </c>
       <c r="I110" t="n">
         <v>12.0</v>
+      </c>
+      <c r="J110" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="111">
@@ -3656,28 +3992,31 @@
         <v>110.0</v>
       </c>
       <c r="B111" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C111" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D111" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E111" t="n">
         <v>96.0</v>
       </c>
       <c r="F111" t="n">
-        <v>9.0</v>
+        <v>12.0</v>
       </c>
       <c r="G111" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="H111" t="n">
         <v>6.0</v>
       </c>
       <c r="I111" t="n">
         <v>12.0</v>
+      </c>
+      <c r="J111" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="112">
@@ -3685,28 +4024,31 @@
         <v>111.0</v>
       </c>
       <c r="B112" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C112" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D112" t="s">
-        <v>29</v>
+        <v>129</v>
       </c>
       <c r="E112" t="n">
         <v>96.0</v>
       </c>
       <c r="F112" t="n">
-        <v>26.0</v>
+        <v>9.0</v>
       </c>
       <c r="G112" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H112" t="n">
         <v>6.0</v>
       </c>
       <c r="I112" t="n">
         <v>12.0</v>
+      </c>
+      <c r="J112" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="113">
@@ -3714,19 +4056,19 @@
         <v>112.0</v>
       </c>
       <c r="B113" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C113" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D113" t="s">
-        <v>128</v>
+        <v>31</v>
       </c>
       <c r="E113" t="n">
         <v>96.0</v>
       </c>
       <c r="F113" t="n">
-        <v>4.0</v>
+        <v>26.0</v>
       </c>
       <c r="G113" t="n">
         <v>0.0</v>
@@ -3736,6 +4078,9 @@
       </c>
       <c r="I113" t="n">
         <v>12.0</v>
+      </c>
+      <c r="J113" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="114">
@@ -3743,19 +4088,19 @@
         <v>113.0</v>
       </c>
       <c r="B114" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C114" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D114" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E114" t="n">
         <v>96.0</v>
       </c>
       <c r="F114" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="G114" t="n">
         <v>0.0</v>
@@ -3765,6 +4110,9 @@
       </c>
       <c r="I114" t="n">
         <v>12.0</v>
+      </c>
+      <c r="J114" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="115">
@@ -3772,28 +4120,31 @@
         <v>114.0</v>
       </c>
       <c r="B115" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C115" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D115" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E115" t="n">
         <v>96.0</v>
       </c>
       <c r="F115" t="n">
-        <v>23.0</v>
+        <v>3.0</v>
       </c>
       <c r="G115" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H115" t="n">
         <v>6.0</v>
       </c>
       <c r="I115" t="n">
         <v>12.0</v>
+      </c>
+      <c r="J115" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="116">
@@ -3801,28 +4152,31 @@
         <v>115.0</v>
       </c>
       <c r="B116" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C116" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D116" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E116" t="n">
         <v>96.0</v>
       </c>
       <c r="F116" t="n">
-        <v>17.0</v>
+        <v>23.0</v>
       </c>
       <c r="G116" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H116" t="n">
         <v>6.0</v>
       </c>
       <c r="I116" t="n">
         <v>12.0</v>
+      </c>
+      <c r="J116" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="117">
@@ -3830,28 +4184,31 @@
         <v>116.0</v>
       </c>
       <c r="B117" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C117" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="D117" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="E117" t="n">
-        <v>64.0</v>
+        <v>96.0</v>
       </c>
       <c r="F117" t="n">
-        <v>4.0</v>
+        <v>17.0</v>
       </c>
       <c r="G117" t="n">
         <v>0.0</v>
       </c>
       <c r="H117" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="I117" t="n">
-        <v>4.0</v>
+        <v>12.0</v>
+      </c>
+      <c r="J117" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="118">
@@ -3859,19 +4216,19 @@
         <v>117.0</v>
       </c>
       <c r="B118" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C118" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D118" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E118" t="n">
         <v>64.0</v>
       </c>
       <c r="F118" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="G118" t="n">
         <v>0.0</v>
@@ -3881,6 +4238,9 @@
       </c>
       <c r="I118" t="n">
         <v>4.0</v>
+      </c>
+      <c r="J118" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="119">
@@ -3888,28 +4248,31 @@
         <v>118.0</v>
       </c>
       <c r="B119" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C119" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D119" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E119" t="n">
         <v>64.0</v>
       </c>
       <c r="F119" t="n">
-        <v>23.0</v>
+        <v>3.0</v>
       </c>
       <c r="G119" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H119" t="n">
         <v>1.0</v>
       </c>
       <c r="I119" t="n">
         <v>4.0</v>
+      </c>
+      <c r="J119" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="120">
@@ -3917,28 +4280,63 @@
         <v>119.0</v>
       </c>
       <c r="B120" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C120" t="s">
+        <v>134</v>
+      </c>
+      <c r="D120" t="s">
         <v>132</v>
-      </c>
-      <c r="D120" t="s">
-        <v>131</v>
       </c>
       <c r="E120" t="n">
         <v>64.0</v>
       </c>
       <c r="F120" t="n">
-        <v>17.0</v>
+        <v>23.0</v>
       </c>
       <c r="G120" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H120" t="n">
         <v>1.0</v>
       </c>
       <c r="I120" t="n">
         <v>4.0</v>
+      </c>
+      <c r="J120" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>120.0</v>
+      </c>
+      <c r="B121" t="s">
+        <v>118</v>
+      </c>
+      <c r="C121" t="s">
+        <v>134</v>
+      </c>
+      <c r="D121" t="s">
+        <v>133</v>
+      </c>
+      <c r="E121" t="n">
+        <v>64.0</v>
+      </c>
+      <c r="F121" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="G121" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H121" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I121" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="J121" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merged team-rocket and power-rangers-rangers
</commit_message>
<xml_diff>
--- a/ES-2Sem-2021-Grupo-5_metricas.xlsx
+++ b/ES-2Sem-2021-Grupo-5_metricas.xlsx
@@ -159,19 +159,19 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="F2" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="G2" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="I2" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="J2" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Total merge, JavaDocs generated
</commit_message>
<xml_diff>
--- a/ES-2Sem-2021-Grupo-5_metricas.xlsx
+++ b/ES-2Sem-2021-Grupo-5_metricas.xlsx
@@ -159,16 +159,16 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="F2" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G2" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="H2" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="I2" t="n">
         <v>3.0</v>

</xml_diff>

<commit_message>
JavaDocs updated and generated
</commit_message>
<xml_diff>
--- a/ES-2Sem-2021-Grupo-5_metricas.xlsx
+++ b/ES-2Sem-2021-Grupo-5_metricas.xlsx
@@ -159,16 +159,16 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F2" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G2" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="H2" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="I2" t="n">
         <v>3.0</v>

</xml_diff>